<commit_message>
Update formdefs and properties.csvs
</commit_message>
<xml_diff>
--- a/app/config/tables/refrigerators/forms/refrigerators/refrigerators.xlsx
+++ b/app/config/tables/refrigerators/forms/refrigerators/refrigerators.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="130">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -320,6 +320,12 @@
     <t xml:space="preserve">auxillaryHash</t>
   </si>
   <si>
+    <t xml:space="preserve">newRowInitialElementKeyToValueMap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">openRowInitialElementKeyToValueMap</t>
+  </si>
+  <si>
     <t xml:space="preserve">linked_table</t>
   </si>
   <si>
@@ -333,6 +339,9 @@
   </si>
   <si>
     <t xml:space="preserve">'catalog_id&gt;='+opendatakit.encodeURIValue(0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{}</t>
   </si>
   <si>
     <t xml:space="preserve">health_facility</t>
@@ -439,16 +448,16 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -476,7 +485,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -500,21 +509,17 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -522,47 +527,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -571,15 +560,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal 2" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Normal 3" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -651,20 +639,20 @@
   </sheetPr>
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.4132653061224"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.4489795918367"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.2091836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.7295918367347"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="41.6122448979592"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.6938775510204"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.4132653061224"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="41.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="32.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -709,7 +697,7 @@
       <c r="A3" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="3" t="n">
+      <c r="B3" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C3" s="2"/>
@@ -885,24 +873,26 @@
   </sheetPr>
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.2091836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.1071428571429"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="44.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -961,58 +951,58 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" s="7" customFormat="true" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
+    <row r="8" s="5" customFormat="true" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="9" s="7" customFormat="true" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
+    <row r="9" s="5" customFormat="true" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="10" s="7" customFormat="true" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
+    <row r="10" s="5" customFormat="true" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="11" s="7" customFormat="true" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
+    <row r="11" s="5" customFormat="true" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="12" s="7" customFormat="true" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
+    <row r="12" s="5" customFormat="true" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="2" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1188,90 +1178,110 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
+  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="22.8214285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="21.4030612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="8" width="17.8265306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="19.5"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="8" width="17.4744897959184"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="8" width="19.3775510204082"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="8" width="39.5867346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="8" width="10.8163265306122"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="39.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="39.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="42.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="10.82"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="7" t="s">
         <v>97</v>
       </c>
+      <c r="H1" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="E2" s="11" t="s">
+      <c r="B2" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="C2" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="D2" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>102</v>
       </c>
+      <c r="F2" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="C3" s="8" t="s">
+      <c r="B3" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="I3" s="0" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1293,83 +1303,83 @@
   </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
+  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="13" width="10.8163265306122"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="34.4744897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="13" width="10.8163265306122"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="9" width="10.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="9" width="34.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="9" width="10.82"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="D1" s="13" t="s">
+      <c r="A1" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="13" t="s">
-        <v>109</v>
+      <c r="E1" s="9" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="D2" s="13" t="s">
+      <c r="A2" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="B2" s="9" t="s">
         <v>114</v>
       </c>
+      <c r="C2" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="D3" s="13" t="s">
+      <c r="A3" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="B3" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>116</v>
       </c>
+      <c r="E3" s="9" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="D4" s="13" t="s">
+      <c r="A4" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="E4" s="13" t="s">
-        <v>118</v>
+      <c r="B4" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1390,48 +1400,48 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.984693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.9387755102041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.4132653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.4132653061224"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="14" t="s">
-        <v>119</v>
+      <c r="A1" s="10" t="s">
+        <v>122</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>20160728</v>
@@ -1439,10 +1449,10 @@
     </row>
     <row r="5" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update xlsx again, add filtering
</commit_message>
<xml_diff>
--- a/app/config/tables/refrigerators/forms/refrigerators/refrigerators.xlsx
+++ b/app/config/tables/refrigerators/forms/refrigerators/refrigerators.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="235">
   <si>
     <t xml:space="preserve">comments</t>
   </si>
@@ -182,13 +182,16 @@
     <t xml:space="preserve">end if</t>
   </si>
   <si>
+    <t xml:space="preserve">model_row_id</t>
+  </si>
+  <si>
     <t xml:space="preserve">assign</t>
   </si>
   <si>
-    <t xml:space="preserve">model_row_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(function() {if (data('common_models') === 'other') { return data('model_other'); } return data('common_models');})()</t>
+    <t xml:space="preserve">model_row_id_wtf_xlsxgenerator_stop_that</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(function() {var x = 0; if (data('common_models') === 'other') { x = data('model_other'); } else { x = data('common_models');}; assign('model_row_id', x); })()</t>
   </si>
   <si>
     <t xml:space="preserve">tracking_id</t>
@@ -968,10 +971,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N18" activeCellId="0" sqref="N18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N22" activeCellId="0" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1258,199 +1261,225 @@
     </row>
     <row r="16" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>35</v>
+        <v>47</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0" t="s">
+      <c r="D17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-    </row>
-    <row r="18" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D18" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="0" t="s">
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D21" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="N18" s="0" t="s">
+      <c r="E21" s="3"/>
+      <c r="F21" s="0" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D19" s="3" t="s">
+      <c r="N21" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D22" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E19" s="3"/>
-      <c r="F19" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="G19" s="0" t="s">
+      <c r="E22" s="3"/>
+      <c r="F22" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="H19" s="0" t="s">
+      <c r="G22" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="I19" s="0" t="s">
+      <c r="H22" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="J19" s="0" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D20" s="3" t="s">
+      <c r="I22" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="0" t="s">
+      <c r="J22" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D23" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G20" s="0" t="s">
+      <c r="E23" s="3"/>
+      <c r="F23" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="H20" s="0" t="s">
+      <c r="G23" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="I20" s="0" t="s">
+      <c r="H23" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="J20" s="0" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D21" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E21" s="0" t="s">
+      <c r="I23" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="F21" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="G21" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="H21" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="I21" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="J21" s="0" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="0" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B23" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="J23" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D24" s="0" t="s">
         <v>41</v>
       </c>
       <c r="E24" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="I24" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="F24" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="G24" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="H24" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="I24" s="0" t="s">
-        <v>73</v>
-      </c>
       <c r="J24" s="0" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D25" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="F25" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="G25" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="H25" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="I25" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="J25" s="0" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D26" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="F26" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="G26" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="H26" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="I26" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="J26" s="0" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B25" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B26" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D27" s="0" t="s">
         <v>41</v>
       </c>
       <c r="E27" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="I27" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="J27" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D28" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="I28" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="J28" s="0" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D29" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="G29" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="H29" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="I29" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="J29" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D30" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="E30" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="G27" s="0" t="s">
+      <c r="F30" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="H27" s="0" t="s">
+      <c r="G30" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="I27" s="0" t="s">
+      <c r="H30" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="J27" s="0" t="s">
+      <c r="I30" s="0" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B28" s="0" t="s">
+      <c r="J30" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B31" s="0" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1486,10 +1515,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>6</v>
@@ -1500,338 +1529,338 @@
     </row>
     <row r="2" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" s="4" customFormat="true" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" s="4" customFormat="true" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" s="4" customFormat="true" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" s="4" customFormat="true" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" s="4" customFormat="true" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1839,13 +1868,13 @@
         <v>42</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1853,13 +1882,13 @@
         <v>42</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1867,13 +1896,13 @@
         <v>42</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1881,13 +1910,13 @@
         <v>42</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1895,13 +1924,13 @@
         <v>42</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1909,13 +1938,13 @@
         <v>42</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -1956,37 +1985,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1994,30 +2023,30 @@
         <v>49</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
       <c r="I2" s="4" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2025,30 +2054,30 @@
         <v>36</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
       <c r="I3" s="4" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="90.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2056,19 +2085,19 @@
         <v>21</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="102.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2076,19 +2105,19 @@
         <v>25</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="102.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2096,19 +2125,19 @@
         <v>30</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -2142,70 +2171,70 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="12" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="12" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -2240,10 +2269,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>6</v>
@@ -2252,31 +2281,31 @@
         <v>7</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>222</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>20170719</v>
@@ -2284,18 +2313,18 @@
     </row>
     <row r="5" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>15</v>
@@ -2303,24 +2332,24 @@
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update xlsx again, fix filtering
</commit_message>
<xml_diff>
--- a/app/config/tables/refrigerators/forms/refrigerators/refrigerators.xlsx
+++ b/app/config/tables/refrigerators/forms/refrigerators/refrigerators.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="234">
   <si>
     <t xml:space="preserve">comments</t>
   </si>
@@ -146,9 +146,6 @@
     <t xml:space="preserve">Facilidad de Salúd</t>
   </si>
   <si>
-    <t xml:space="preserve">choice_item.admin_region === data('adminRegion')</t>
-  </si>
-  <si>
     <t xml:space="preserve">select_one</t>
   </si>
   <si>
@@ -170,7 +167,7 @@
     <t xml:space="preserve">if</t>
   </si>
   <si>
-    <t xml:space="preserve">data('common_models') === 'other'</t>
+    <t xml:space="preserve">data('models_common') === 'other'</t>
   </si>
   <si>
     <t xml:space="preserve">refrigerator_model_list</t>
@@ -182,16 +179,13 @@
     <t xml:space="preserve">end if</t>
   </si>
   <si>
+    <t xml:space="preserve">assign</t>
+  </si>
+  <si>
     <t xml:space="preserve">model_row_id</t>
   </si>
   <si>
-    <t xml:space="preserve">assign</t>
-  </si>
-  <si>
-    <t xml:space="preserve">model_row_id_wtf_xlsxgenerator_stop_that</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(function() {var x = 0; if (data('common_models') === 'other') { x = data('model_other'); } else { x = data('common_models');}; assign('model_row_id', x); })()</t>
+    <t xml:space="preserve">(function() {if (data('models_common') === 'other') { return data('model_other'); } return data('models_common');})()</t>
   </si>
   <si>
     <t xml:space="preserve">tracking_id</t>
@@ -617,7 +611,10 @@
     <t xml:space="preserve">health_facility</t>
   </si>
   <si>
-    <t xml:space="preserve">facility_id &gt;= ?</t>
+    <t xml:space="preserve">admin_region = ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[data('adminRegion')]</t>
   </si>
   <si>
     <t xml:space="preserve">'facility_id&gt;='+opendatakit.encodeURIValue(0)</t>
@@ -973,8 +970,8 @@
   </sheetPr>
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N22" activeCellId="0" sqref="N22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K9" activeCellId="0" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1176,9 +1173,6 @@
       <c r="J9" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="M9" s="0" t="s">
-        <v>40</v>
-      </c>
     </row>
     <row r="10" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="5"/>
@@ -1198,97 +1192,83 @@
     </row>
     <row r="12" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="F12" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="F12" s="0" t="s">
+      <c r="G12" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="G12" s="0" t="s">
+      <c r="H12" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="H12" s="0" t="s">
+      <c r="I12" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="I12" s="0" t="s">
-        <v>46</v>
-      </c>
       <c r="J12" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="0" t="s">
         <v>47</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>48</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D14" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E14" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="F14" s="0" t="s">
-        <v>50</v>
-      </c>
       <c r="G14" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H14" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="H14" s="0" t="s">
+      <c r="I14" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="I14" s="0" t="s">
-        <v>46</v>
-      </c>
       <c r="J14" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="0" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D17" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="D17" s="3"/>
       <c r="E17" s="3"/>
-      <c r="F17" s="0" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="18" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B18" s="0" t="s">
-        <v>51</v>
-      </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
     </row>
     <row r="19" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B19" s="0" t="s">
-        <v>35</v>
-      </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
     </row>
@@ -1301,14 +1281,14 @@
     </row>
     <row r="21" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D21" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="0" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="N21" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1317,63 +1297,63 @@
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="H22" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="G22" s="0" t="s">
+      <c r="I22" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="H22" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="I22" s="0" t="s">
-        <v>59</v>
-      </c>
       <c r="J22" s="0" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D23" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="H23" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="G23" s="0" t="s">
+      <c r="I23" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="H23" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="I23" s="0" t="s">
-        <v>64</v>
-      </c>
       <c r="J23" s="0" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D24" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E24" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="G24" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="F24" s="0" t="s">
+      <c r="H24" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="G24" s="0" t="s">
+      <c r="I24" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="H24" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="I24" s="0" t="s">
-        <v>69</v>
-      </c>
       <c r="J24" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1388,94 +1368,94 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D27" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E27" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="G27" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="F27" s="0" t="s">
+      <c r="H27" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="G27" s="0" t="s">
+      <c r="I27" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="H27" s="0" t="s">
+      <c r="J27" s="0" t="s">
         <v>73</v>
-      </c>
-      <c r="I27" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="J27" s="0" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D28" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E28" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="G28" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="F28" s="0" t="s">
+      <c r="H28" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="G28" s="0" t="s">
+      <c r="I28" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="H28" s="0" t="s">
+      <c r="J28" s="0" t="s">
         <v>79</v>
-      </c>
-      <c r="I28" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J28" s="0" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D29" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E29" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="G29" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="F29" s="0" t="s">
+      <c r="H29" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="G29" s="0" t="s">
+      <c r="I29" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="H29" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="I29" s="0" t="s">
-        <v>86</v>
-      </c>
       <c r="J29" s="0" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D30" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E30" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G30" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="H30" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="G30" s="0" t="s">
+      <c r="I30" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="H30" s="0" t="s">
+      <c r="J30" s="0" t="s">
         <v>90</v>
-      </c>
-      <c r="I30" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="J30" s="0" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1502,7 +1482,7 @@
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D52" activeCellId="0" sqref="D52"/>
+      <selection pane="topLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1515,10 +1495,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>6</v>
@@ -1529,422 +1509,422 @@
     </row>
     <row r="2" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>96</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>99</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>102</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>105</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" s="4" customFormat="true" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>110</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="9" s="4" customFormat="true" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="10" s="4" customFormat="true" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>116</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="11" s="4" customFormat="true" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>119</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="12" s="4" customFormat="true" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>122</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B15" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D15" s="0" t="s">
         <v>127</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B16" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D16" s="0" t="s">
         <v>130</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B18" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="D18" s="0" t="s">
         <v>133</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B19" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="D19" s="0" t="s">
         <v>136</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B20" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="D20" s="0" t="s">
         <v>139</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B21" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="D21" s="0" t="s">
         <v>142</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B22" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D22" s="0" t="s">
         <v>145</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="C24" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="B24" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>72</v>
-      </c>
       <c r="D24" s="0" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B25" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="D25" s="0" t="s">
         <v>150</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B26" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="D26" s="0" t="s">
         <v>153</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B28" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D28" s="0" t="s">
         <v>156</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B30" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="D30" s="0" t="s">
         <v>122</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="D30" s="0" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B33" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="D33" s="0" t="s">
         <v>161</v>
-      </c>
-      <c r="C33" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="D33" s="0" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B34" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="D34" s="0" t="s">
         <v>164</v>
-      </c>
-      <c r="C34" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="D34" s="0" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B35" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="D35" s="0" t="s">
         <v>167</v>
-      </c>
-      <c r="C35" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="D35" s="0" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B36" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="D36" s="0" t="s">
         <v>170</v>
-      </c>
-      <c r="C36" s="0" t="s">
-        <v>171</v>
-      </c>
-      <c r="D36" s="0" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B37" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="D37" s="0" t="s">
         <v>173</v>
-      </c>
-      <c r="C37" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="D37" s="0" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B38" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="D38" s="0" t="s">
         <v>176</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>177</v>
-      </c>
-      <c r="D38" s="0" t="s">
-        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -1966,7 +1946,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1985,68 +1965,68 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="J1" s="0" t="s">
         <v>186</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="K1" s="0" t="s">
         <v>187</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="K1" s="0" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="F2" s="10" t="s">
         <v>191</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>191</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>193</v>
       </c>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
       <c r="I2" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2054,30 +2034,30 @@
         <v>36</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>196</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>193</v>
       </c>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
       <c r="I3" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="90.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2085,19 +2065,19 @@
         <v>21</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="G4" s="0" t="s">
         <v>199</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="H4" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="H4" s="11" t="s">
-        <v>201</v>
-      </c>
       <c r="J4" s="0" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="102.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2105,19 +2085,19 @@
         <v>25</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="G5" s="0" t="s">
         <v>199</v>
       </c>
-      <c r="G5" s="0" t="s">
-        <v>200</v>
-      </c>
       <c r="H5" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="102.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2125,19 +2105,19 @@
         <v>30</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G6" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="H6" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="H6" s="11" t="s">
-        <v>204</v>
-      </c>
       <c r="J6" s="0" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -2171,70 +2151,70 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="C1" s="12" t="s">
         <v>206</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>207</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>209</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="C2" s="12" t="s">
         <v>210</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="D2" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="E2" s="12" t="s">
         <v>212</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>209</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>210</v>
-      </c>
       <c r="C3" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="E3" s="12" t="s">
         <v>214</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>209</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>210</v>
-      </c>
       <c r="C4" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="E4" s="12" t="s">
         <v>216</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -2255,7 +2235,7 @@
   </sheetPr>
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -2269,10 +2249,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>6</v>
@@ -2281,50 +2261,50 @@
         <v>7</v>
       </c>
       <c r="E1" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="F1" s="0" t="s">
         <v>219</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>221</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>20170719</v>
+        <v>20170720</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="0" t="s">
         <v>226</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>15</v>
@@ -2332,24 +2312,24 @@
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>229</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="F7" s="0" t="s">
         <v>230</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>232</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="F8" s="0" t="s">
         <v>233</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix model_row_id by adding it to the model in the xlsx
</commit_message>
<xml_diff>
--- a/app/config/tables/refrigerators/forms/refrigerators/refrigerators.xlsx
+++ b/app/config/tables/refrigerators/forms/refrigerators/refrigerators.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,6 +13,7 @@
     <sheet name="queries" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="properties" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="settings" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="model" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="234">
   <si>
     <t xml:space="preserve">comments</t>
   </si>
@@ -2235,7 +2236,7 @@
   </sheetPr>
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -2341,4 +2342,47 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"DejaVu Serif,Book"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"DejaVu Serif,Book"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Make Richard's requested changes
</commit_message>
<xml_diff>
--- a/app/config/tables/refrigerators/forms/refrigerators/refrigerators.xlsx
+++ b/app/config/tables/refrigerators/forms/refrigerators/refrigerators.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="231">
   <si>
     <t xml:space="preserve">comments</t>
   </si>
@@ -69,6 +69,15 @@
     <t xml:space="preserve">calculation</t>
   </si>
   <si>
+    <t xml:space="preserve">required</t>
+  </si>
+  <si>
+    <t xml:space="preserve">begin screen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if</t>
+  </si>
+  <si>
     <t xml:space="preserve">text</t>
   </si>
   <si>
@@ -84,7 +93,7 @@
     <t xml:space="preserve">Enter refrigerator ID:</t>
   </si>
   <si>
-    <t xml:space="preserve">begin screen</t>
+    <t xml:space="preserve">end if</t>
   </si>
   <si>
     <t xml:space="preserve">select_one_dropdown</t>
@@ -165,9 +174,6 @@
     <t xml:space="preserve">Choose the refrigerator model:</t>
   </si>
   <si>
-    <t xml:space="preserve">if</t>
-  </si>
-  <si>
     <t xml:space="preserve">data('models_common') === 'other'</t>
   </si>
   <si>
@@ -177,16 +183,43 @@
     <t xml:space="preserve">model_other</t>
   </si>
   <si>
-    <t xml:space="preserve">end if</t>
-  </si>
-  <si>
     <t xml:space="preserve">assign</t>
   </si>
   <si>
     <t xml:space="preserve">model_row_id</t>
   </si>
   <si>
-    <t xml:space="preserve">(function() {if (data('models_common') === 'other') { return data('model_other'); } return data('models_common');})()</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(function() {</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (data('models_common') === 'other') { return data('model_other'); } return data('models_common');})()</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">tracking_id</t>
@@ -201,7 +234,10 @@
     <t xml:space="preserve">Enter the tracking ID: </t>
   </si>
   <si>
-    <t xml:space="preserve">number</t>
+    <t xml:space="preserve">select_one_integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">years</t>
   </si>
   <si>
     <t xml:space="preserve">year</t>
@@ -504,49 +540,34 @@
     <t xml:space="preserve">No</t>
   </si>
   <si>
-    <t xml:space="preserve">M5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Common Model Name One</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nombre del Modelo Popular Uno</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Common Model Name Two</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nombre del Modelo Popular Dos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Common Model Name Three</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nombre del Modelo Popular Tres</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Common Model Name Four</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nombre del Modelo Popular Quatro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Common Model Name Five</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nombre del Modelo Popular Cinco</t>
+    <t xml:space="preserve">M51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V 170 GE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GBC-340</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V 170 EK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MK304</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RCW 50 EK</t>
   </si>
   <si>
     <t xml:space="preserve">other</t>
@@ -738,7 +759,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -766,6 +787,14 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -829,7 +858,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -867,23 +896,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -969,10 +998,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N31"/>
+  <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K9" activeCellId="0" sqref="K9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -985,8 +1014,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="29.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="30.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="41.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="32.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="12.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="32.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="9.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="6.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="11.41"/>
   </cols>
   <sheetData>
@@ -1033,239 +1063,269 @@
       <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="0" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D2" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="B2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="3"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>19</v>
+        <v>16</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="I4" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="J4" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="D5" s="3"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D6" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="E6" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="F6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D7" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D5" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="0" t="s">
+      <c r="E7" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="M5" s="0" t="s">
+      <c r="F7" s="0" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="23.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5"/>
-      <c r="D6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="0" t="s">
+      <c r="G7" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="H7" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="I7" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="M7" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="0" t="s">
+      <c r="O7" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="23.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5"/>
+      <c r="D8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="J6" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="L6" s="6"/>
-      <c r="M6" s="0" t="s">
+      <c r="F8" s="0" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="23.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5"/>
-      <c r="B7" s="0" t="s">
+      <c r="G8" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="L7" s="6"/>
-    </row>
-    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D9" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="0" t="s">
+      <c r="H8" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="I8" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="L8" s="6"/>
+      <c r="M8" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="G9" s="0" t="s">
+      <c r="O8" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="23.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5"/>
+      <c r="B9" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="H9" s="0" t="s">
+      <c r="D9" s="3"/>
+      <c r="L9" s="6"/>
+    </row>
+    <row r="10" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D11" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="I9" s="0" t="s">
+      <c r="F11" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="O11" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5"/>
+      <c r="B12" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="J9" s="0" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5"/>
-      <c r="B10" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="L10" s="6"/>
-    </row>
-    <row r="11" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5"/>
-      <c r="B11" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="L11" s="6"/>
-    </row>
-    <row r="12" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="G12" s="0" t="s">
+      <c r="D12" s="3"/>
+      <c r="L12" s="6"/>
+    </row>
+    <row r="13" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5"/>
+      <c r="B13" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="L13" s="6"/>
+    </row>
+    <row r="14" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D14" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H12" s="0" t="s">
+      <c r="E14" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="I12" s="0" t="s">
+      <c r="F14" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="J12" s="0" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0" t="s">
+      <c r="G14" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="H14" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D14" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="3" t="s">
+      <c r="I14" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="F14" s="0" t="s">
+      <c r="J14" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="O14" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="0" t="s">
         <v>49</v>
-      </c>
-      <c r="G14" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="H14" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="I14" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="J14" s="0" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0" t="s">
-        <v>50</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="I16" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="J16" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="O16" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B17" s="0" t="s">
+        <v>22</v>
+      </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0" t="s">
+        <v>38</v>
+      </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
     </row>
@@ -1274,194 +1334,204 @@
       <c r="E19" s="3"/>
     </row>
     <row r="20" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="0" t="s">
-        <v>19</v>
-      </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
     <row r="21" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D21" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="D21" s="3"/>
       <c r="E21" s="3"/>
-      <c r="F21" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="N21" s="0" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="22" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D22" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="B22" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="3"/>
       <c r="E22" s="3"/>
-      <c r="F22" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="G22" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="H22" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="I22" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="J22" s="0" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="23" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D23" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="N23" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D24" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="F24" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="I24" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="J24" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D25" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="G23" s="0" t="s">
+      <c r="E25" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H23" s="0" t="s">
+      <c r="F25" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="I23" s="0" t="s">
+      <c r="G25" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="J23" s="0" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D24" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="E24" s="0" t="s">
+      <c r="H25" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="F24" s="0" t="s">
+      <c r="I25" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="G24" s="0" t="s">
+      <c r="J25" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D26" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="H24" s="0" t="s">
+      <c r="F26" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="I24" s="0" t="s">
+      <c r="G26" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="J24" s="0" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B25" s="0" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B26" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D27" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="E27" s="0" t="s">
+      <c r="H26" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="F27" s="0" t="s">
+      <c r="I26" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="G27" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="H27" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="I27" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="J27" s="0" t="s">
-        <v>73</v>
+      <c r="J26" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B27" s="0" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D28" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="F28" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="G28" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="H28" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="I28" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="J28" s="0" t="s">
-        <v>79</v>
+      <c r="B28" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D29" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E29" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="G29" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="H29" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="I29" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="J29" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D30" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="H30" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="I30" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="F29" s="0" t="s">
+      <c r="J30" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="G29" s="0" t="s">
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D31" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="H29" s="0" t="s">
+      <c r="F31" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="I29" s="0" t="s">
+      <c r="G31" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="J29" s="0" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D30" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="E30" s="0" t="s">
+      <c r="H31" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="I31" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="G30" s="0" t="s">
+      <c r="J31" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D32" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E32" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="H30" s="0" t="s">
+      <c r="F32" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="I30" s="0" t="s">
+      <c r="G32" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="J30" s="0" t="s">
+      <c r="H32" s="0" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B31" s="0" t="s">
-        <v>35</v>
+      <c r="I32" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="J32" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B33" s="0" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1480,10 +1550,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B38" activeCellId="0" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1496,10 +1566,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>6</v>
@@ -1510,363 +1580,363 @@
     </row>
     <row r="2" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" s="4" customFormat="true" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" s="4" customFormat="true" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" s="4" customFormat="true" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" s="4" customFormat="true" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" s="4" customFormat="true" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>164</v>
@@ -1874,7 +1944,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B35" s="0" t="s">
         <v>165</v>
@@ -1883,49 +1953,301 @@
         <v>166</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B36" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="C36" s="0" t="s">
         <v>168</v>
       </c>
-      <c r="C36" s="0" t="s">
-        <v>169</v>
-      </c>
       <c r="D36" s="0" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>176</v>
+        <v>173</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>2016</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>2016</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>2015</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>2015</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>2014</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>2014</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>2013</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>2013</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>2012</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <v>2011</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <v>2011</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>2010</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <v>2010</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>2009</v>
+      </c>
+      <c r="C48" s="0" t="n">
+        <v>2009</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B49" s="0" t="n">
+        <v>2008</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>2008</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>2007</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <v>2007</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>2006</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <v>2006</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B52" s="0" t="n">
+        <v>2005</v>
+      </c>
+      <c r="C52" s="0" t="n">
+        <v>2005</v>
+      </c>
+      <c r="D52" s="0" t="n">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B53" s="0" t="n">
+        <v>2004</v>
+      </c>
+      <c r="C53" s="0" t="n">
+        <v>2004</v>
+      </c>
+      <c r="D53" s="0" t="n">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B54" s="0" t="n">
+        <v>2003</v>
+      </c>
+      <c r="C54" s="0" t="n">
+        <v>2003</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B55" s="0" t="n">
+        <v>2002</v>
+      </c>
+      <c r="C55" s="0" t="n">
+        <v>2002</v>
+      </c>
+      <c r="D55" s="0" t="n">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B56" s="0" t="n">
+        <v>2001</v>
+      </c>
+      <c r="C56" s="0" t="n">
+        <v>2001</v>
+      </c>
+      <c r="D56" s="0" t="n">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B57" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="C57" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <v>2000</v>
       </c>
     </row>
   </sheetData>
@@ -1966,159 +2288,159 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="E1" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="J1" s="0" t="s">
         <v>183</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="K1" s="0" t="s">
         <v>184</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>186</v>
-      </c>
-      <c r="K1" s="0" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>188</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>189</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>189</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>191</v>
       </c>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
       <c r="I2" s="4" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
       <c r="I3" s="4" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="90.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="102.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="H5" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="G5" s="0" t="s">
-        <v>199</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>201</v>
-      </c>
       <c r="J5" s="0" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="102.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -2152,70 +2474,70 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="D2" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="E2" s="12" t="s">
         <v>209</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>210</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>211</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>209</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>213</v>
-      </c>
-      <c r="D3" s="12" t="s">
+      <c r="E3" s="12" t="s">
         <v>211</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="D4" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>209</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>215</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>211</v>
-      </c>
       <c r="E4" s="12" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -2236,7 +2558,7 @@
   </sheetPr>
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -2250,10 +2572,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>6</v>
@@ -2262,75 +2584,75 @@
         <v>7</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>20170720</v>
+        <v>20170721</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -2351,7 +2673,7 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -2370,10 +2692,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update xlsx, but not CSVs yet
</commit_message>
<xml_diff>
--- a/app/config/tables/refrigerators/forms/refrigerators/refrigerators.xlsx
+++ b/app/config/tables/refrigerators/forms/refrigerators/refrigerators.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="221">
   <si>
     <t xml:space="preserve">comments</t>
   </si>
@@ -96,64 +96,25 @@
     <t xml:space="preserve">end if</t>
   </si>
   <si>
+    <t xml:space="preserve">data('facility_row_id') == null</t>
+  </si>
+  <si>
     <t xml:space="preserve">select_one_dropdown</t>
   </si>
   <si>
-    <t xml:space="preserve">regionLevel1_csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">regionLevel1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Level 1 of admin region</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nievel Uno de Región de Administracion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">regionLevel2_csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">regionLevel2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Level 2 of admin region</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nievel Dos de Región de Administracion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">choice_item.regionLevel1 === data('regionLevel1')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">regionLevel3_csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">adminRegion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Admin region</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Región de Administracion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">choice_item.regionLevel2 === data('regionLevel2')</t>
+    <t xml:space="preserve">health_facility_list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">facility_row_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Health Facility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Facilidad de Salúd</t>
   </si>
   <si>
     <t xml:space="preserve">end screen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">health_facility_list</t>
-  </si>
-  <si>
-    <t xml:space="preserve">facility_row_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Health Facility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Facilidad de Salúd</t>
   </si>
   <si>
     <t xml:space="preserve">select_one</t>
@@ -642,6 +603,9 @@
     <t xml:space="preserve">'facility_id&gt;='+opendatakit.encodeURIValue(0)</t>
   </si>
   <si>
+    <t xml:space="preserve">regionLevel1_csv</t>
+  </si>
+  <si>
     <t xml:space="preserve">csv</t>
   </si>
   <si>
@@ -651,7 +615,13 @@
     <t xml:space="preserve">_.chain(context).pluck('regionLevel1').uniq().map(function(regionLevel1){ return {name:regionLevel1, label:regionLevel1, data_value:regionLevel1, display:{title: {text:regionLevel1}}}; }).value()</t>
   </si>
   <si>
+    <t xml:space="preserve">regionLevel2_csv</t>
+  </si>
+  <si>
     <t xml:space="preserve">_.map(context, function(place){ place.name = place.regionLevel2; place.label = place.regionLevel2; place.data_value = place.name; place.display = {title: {text:place.label}}; return place; })</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regionLevel3_csv</t>
   </si>
   <si>
     <t xml:space="preserve">"regions2-3.csv"</t>
@@ -1000,8 +970,8 @@
   </sheetPr>
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O25" activeCellId="0" sqref="O25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1113,55 +1083,34 @@
       <c r="E5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D6" s="0" t="s">
+      <c r="B6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>23</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="J6" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="O6" s="0" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D7" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E7" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>31</v>
-      </c>
       <c r="I7" s="0" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="M7" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="O7" s="0" t="n">
         <v>1</v>
@@ -1169,79 +1118,24 @@
     </row>
     <row r="8" customFormat="false" ht="23.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="5"/>
-      <c r="D8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="I8" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="J8" s="0" t="s">
-        <v>36</v>
-      </c>
+      <c r="B8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="3"/>
       <c r="L8" s="6"/>
-      <c r="M8" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="O8" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="9" customFormat="false" ht="23.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="5"/>
       <c r="B9" s="0" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="D9" s="3"/>
       <c r="L9" s="6"/>
     </row>
-    <row r="10" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D11" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="G11" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="I11" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="J11" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="O11" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
+    <row r="10" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="5"/>
-      <c r="B12" s="0" t="s">
-        <v>38</v>
-      </c>
       <c r="D12" s="3"/>
       <c r="L12" s="6"/>
     </row>
@@ -1255,25 +1149,25 @@
     </row>
     <row r="14" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D14" s="3" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="O14" s="0" t="n">
         <v>1</v>
@@ -1284,35 +1178,35 @@
         <v>16</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D16" s="3" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="O16" s="0" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1324,7 +1218,7 @@
     </row>
     <row r="18" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -1350,14 +1244,14 @@
     </row>
     <row r="23" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D23" s="3" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="0" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="N23" s="0" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1366,19 +1260,19 @@
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="0" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="O24" s="0" t="n">
         <v>1</v>
@@ -1386,53 +1280,53 @@
     </row>
     <row r="25" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D25" s="3" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D26" s="0" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1442,99 +1336,99 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D29" s="0" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="J29" s="0" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D30" s="0" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="J30" s="0" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D31" s="0" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="J31" s="0" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D32" s="0" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="J32" s="0" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1555,8 +1449,8 @@
   </sheetPr>
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B38" activeCellId="0" sqref="B38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C38" activeCellId="0" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1569,10 +1463,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>6</v>
@@ -1583,427 +1477,427 @@
     </row>
     <row r="2" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>108</v>
-      </c>
       <c r="C6" s="0" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" s="4" customFormat="true" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" s="4" customFormat="true" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" s="4" customFormat="true" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" s="4" customFormat="true" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" s="4" customFormat="true" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>2017</v>
@@ -2017,7 +1911,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>2016</v>
@@ -2031,7 +1925,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>2015</v>
@@ -2045,7 +1939,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>2014</v>
@@ -2059,7 +1953,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>2013</v>
@@ -2073,7 +1967,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>2012</v>
@@ -2087,7 +1981,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>2011</v>
@@ -2101,7 +1995,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>2010</v>
@@ -2115,7 +2009,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>2009</v>
@@ -2129,7 +2023,7 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>2008</v>
@@ -2143,7 +2037,7 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>2007</v>
@@ -2157,7 +2051,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>2006</v>
@@ -2171,7 +2065,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>2005</v>
@@ -2185,7 +2079,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>2004</v>
@@ -2199,7 +2093,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>2003</v>
@@ -2213,7 +2107,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>2002</v>
@@ -2227,7 +2121,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>2001</v>
@@ -2241,7 +2135,7 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>2000</v>
@@ -2291,159 +2185,159 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
       <c r="I2" s="4" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
       <c r="I3" s="4" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="90.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>24</v>
+        <v>182</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="102.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>28</v>
+        <v>186</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="102.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>33</v>
+        <v>188</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -2465,7 +2359,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2477,70 +2371,70 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="12" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="12" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -2561,7 +2455,7 @@
   </sheetPr>
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -2575,10 +2469,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>6</v>
@@ -2587,31 +2481,31 @@
         <v>7</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>20170724</v>
@@ -2619,43 +2513,43 @@
     </row>
     <row r="5" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -2695,10 +2589,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change year installed to an integer with appropriate constraint
</commit_message>
<xml_diff>
--- a/app/config/tables/refrigerators/forms/refrigerators/refrigerators.xlsx
+++ b/app/config/tables/refrigerators/forms/refrigerators/refrigerators.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clarice\cold-chain\cold-chain-app-designer\app\config\tables\refrigerators\forms\refrigerators\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="37940" windowHeight="19700" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="37935" windowHeight="19695" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -13,8 +18,9 @@
     <sheet name="properties" sheetId="4" r:id="rId4"/>
     <sheet name="settings" sheetId="5" r:id="rId5"/>
     <sheet name="model" sheetId="6" r:id="rId6"/>
+    <sheet name="calculates" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="257">
   <si>
     <t>comments</t>
   </si>
@@ -182,12 +188,6 @@
     <t xml:space="preserve">Enter the tracking ID: </t>
   </si>
   <si>
-    <t>select_one_integer</t>
-  </si>
-  <si>
-    <t>years</t>
-  </si>
-  <si>
     <t>year</t>
   </si>
   <si>
@@ -792,16 +792,59 @@
   </si>
   <si>
     <t>No Aplica</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>constraint</t>
+  </si>
+  <si>
+    <t>display.constraint_message.text</t>
+  </si>
+  <si>
+    <t>calculation_name</t>
+  </si>
+  <si>
+    <t>valid_refrigerator_year</t>
+  </si>
+  <si>
+    <t>calculates.valid_refrigerator_year()</t>
+  </si>
+  <si>
+    <t>display.constraint_message.text.es</t>
+  </si>
+  <si>
+    <t>El año debe ser entre 1950 y el año actual o -1 si se desconoce</t>
+  </si>
+  <si>
+    <t>Year must be between 1950 and the current year or -1 if unknown</t>
+  </si>
+  <si>
+    <t>(function() {
+  var currDate = new Date();
+  var currYear = currDate.getFullYear();
+  return (data('year') &gt;= 1950 &amp;&amp; data('year') &lt;= currYear) || data('year') === -1
+})()</t>
+  </si>
+  <si>
+    <t>display.hint.text.es</t>
+  </si>
+  <si>
+    <t>Enter -1 if year is unknown</t>
+  </si>
+  <si>
+    <t>Ingrese -1 si el año es desconocido</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -843,6 +886,11 @@
       <name val="Arial"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -881,7 +929,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -910,6 +958,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -990,6 +1042,14 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1315,29 +1375,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:S23"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="42.83203125" customWidth="1"/>
-    <col min="2" max="3" width="11.33203125" customWidth="1"/>
-    <col min="4" max="4" width="20.5" customWidth="1"/>
-    <col min="5" max="5" width="25.1640625" customWidth="1"/>
-    <col min="6" max="6" width="24.6640625" customWidth="1"/>
-    <col min="7" max="7" width="29.6640625" customWidth="1"/>
-    <col min="8" max="8" width="30.5" customWidth="1"/>
-    <col min="9" max="9" width="41.6640625" customWidth="1"/>
-    <col min="10" max="10" width="34.83203125" customWidth="1"/>
-    <col min="11" max="11" width="9.5" customWidth="1"/>
-    <col min="12" max="12" width="6.1640625" customWidth="1"/>
-    <col min="13" max="1025" width="11.33203125" customWidth="1"/>
+    <col min="1" max="1" width="42.85546875" customWidth="1"/>
+    <col min="2" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" customWidth="1"/>
+    <col min="7" max="7" width="29.5703125" customWidth="1"/>
+    <col min="8" max="8" width="30.42578125" customWidth="1"/>
+    <col min="9" max="9" width="41.5703125" customWidth="1"/>
+    <col min="10" max="10" width="22.85546875" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" customWidth="1"/>
+    <col min="12" max="12" width="20.28515625" customWidth="1"/>
+    <col min="13" max="13" width="16.140625" customWidth="1"/>
+    <col min="14" max="1026" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1372,26 +1433,38 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
+        <v>254</v>
+      </c>
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" ht="16" customHeight="1">
+      <c r="Q1" s="15" t="s">
+        <v>245</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:15" ht="16" customHeight="1">
+    <row r="3" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>16</v>
       </c>
@@ -1399,7 +1472,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="16" customHeight="1">
+    <row r="4" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D4" t="s">
         <v>18</v>
       </c>
@@ -1421,19 +1494,19 @@
       <c r="J4" t="s">
         <v>22</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="23.25" customHeight="1">
+    <row r="5" spans="1:19" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
       <c r="B5" t="s">
         <v>23</v>
       </c>
       <c r="D5" s="3"/>
-      <c r="L5" s="6"/>
-    </row>
-    <row r="6" spans="1:15" ht="18" customHeight="1">
+      <c r="M5" s="6"/>
+    </row>
+    <row r="6" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D6" s="3" t="s">
         <v>24</v>
       </c>
@@ -1455,11 +1528,11 @@
       <c r="J6" t="s">
         <v>28</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="18" customHeight="1">
+    <row r="7" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>16</v>
       </c>
@@ -1469,7 +1542,7 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:15" ht="16" customHeight="1">
+    <row r="8" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D8" s="3" t="s">
         <v>24</v>
       </c>
@@ -1491,32 +1564,32 @@
       <c r="J8" t="s">
         <v>28</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="16" customHeight="1">
+    <row r="9" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>23</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:15" ht="16" customHeight="1">
+    <row r="10" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>33</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:15" ht="16" customHeight="1">
+    <row r="11" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>15</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:15" ht="16" customHeight="1">
+    <row r="12" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D12" s="3" t="s">
         <v>34</v>
       </c>
@@ -1524,11 +1597,11 @@
       <c r="F12" t="s">
         <v>35</v>
       </c>
-      <c r="N12" t="s">
+      <c r="O12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="16" customHeight="1">
+    <row r="13" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D13" s="3" t="s">
         <v>37</v>
       </c>
@@ -1548,186 +1621,199 @@
       <c r="J13" t="s">
         <v>40</v>
       </c>
-      <c r="O13">
+      <c r="P13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="16" customHeight="1">
+    <row r="14" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D14" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="G14" t="s">
         <v>43</v>
       </c>
-      <c r="F14" t="s">
+      <c r="H14" t="s">
         <v>44</v>
       </c>
-      <c r="G14" t="s">
+      <c r="I14" t="s">
         <v>45</v>
       </c>
-      <c r="H14" t="s">
-        <v>46</v>
-      </c>
-      <c r="I14" t="s">
-        <v>47</v>
-      </c>
       <c r="J14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="16" customHeight="1">
+        <v>44</v>
+      </c>
+      <c r="K14" t="s">
+        <v>255</v>
+      </c>
+      <c r="L14" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>249</v>
+      </c>
+      <c r="R14" t="s">
+        <v>252</v>
+      </c>
+      <c r="S14" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>33</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:15" ht="16" customHeight="1">
+    <row r="16" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>15</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="2:10" ht="16" customHeight="1">
+    <row r="17" spans="2:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D17" t="s">
         <v>24</v>
       </c>
       <c r="E17" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" t="s">
+        <v>47</v>
+      </c>
+      <c r="G17" t="s">
         <v>48</v>
       </c>
-      <c r="F17" t="s">
+      <c r="H17" t="s">
         <v>49</v>
       </c>
-      <c r="G17" t="s">
+      <c r="I17" t="s">
         <v>50</v>
       </c>
-      <c r="H17" t="s">
-        <v>51</v>
-      </c>
-      <c r="I17" t="s">
-        <v>52</v>
-      </c>
       <c r="J17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" ht="15" customHeight="1">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D18" t="s">
         <v>24</v>
       </c>
       <c r="E18" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" t="s">
         <v>53</v>
       </c>
-      <c r="F18" t="s">
+      <c r="H18" t="s">
         <v>54</v>
       </c>
-      <c r="G18" t="s">
+      <c r="I18" t="s">
         <v>55</v>
       </c>
-      <c r="H18" t="s">
+      <c r="J18" t="s">
         <v>56</v>
       </c>
-      <c r="I18" t="s">
-        <v>57</v>
-      </c>
-      <c r="J18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" ht="16" customHeight="1">
+    </row>
+    <row r="19" spans="2:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D19" t="s">
         <v>24</v>
       </c>
       <c r="E19" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" t="s">
+        <v>58</v>
+      </c>
+      <c r="G19" t="s">
         <v>59</v>
       </c>
-      <c r="F19" t="s">
+      <c r="H19" t="s">
         <v>60</v>
       </c>
-      <c r="G19" t="s">
+      <c r="I19" t="s">
         <v>61</v>
       </c>
-      <c r="H19" t="s">
+      <c r="J19" t="s">
         <v>62</v>
       </c>
-      <c r="I19" t="s">
-        <v>63</v>
-      </c>
-      <c r="J19" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" ht="15" customHeight="1">
+    </row>
+    <row r="20" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D20" t="s">
         <v>24</v>
       </c>
       <c r="E20" t="s">
+        <v>63</v>
+      </c>
+      <c r="F20" t="s">
+        <v>64</v>
+      </c>
+      <c r="G20" t="s">
         <v>65</v>
       </c>
-      <c r="F20" t="s">
+      <c r="H20" t="s">
         <v>66</v>
       </c>
-      <c r="G20" t="s">
+      <c r="I20" t="s">
         <v>67</v>
       </c>
-      <c r="H20" t="s">
-        <v>68</v>
-      </c>
-      <c r="I20" t="s">
-        <v>69</v>
-      </c>
       <c r="J20" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" ht="15" customHeight="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D21" t="s">
         <v>24</v>
       </c>
       <c r="E21" t="s">
+        <v>228</v>
+      </c>
+      <c r="F21" t="s">
+        <v>229</v>
+      </c>
+      <c r="G21" t="s">
         <v>230</v>
       </c>
-      <c r="F21" t="s">
+      <c r="H21" t="s">
         <v>231</v>
       </c>
-      <c r="G21" t="s">
+      <c r="I21" t="s">
         <v>232</v>
       </c>
-      <c r="H21" t="s">
+      <c r="J21" t="s">
         <v>233</v>
       </c>
-      <c r="I21" t="s">
-        <v>234</v>
-      </c>
-      <c r="J21" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" ht="12.75" customHeight="1">
+    </row>
+    <row r="22" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D22" t="s">
         <v>24</v>
       </c>
       <c r="E22" t="s">
+        <v>68</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G22" t="s">
         <v>70</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="H22" t="s">
         <v>71</v>
       </c>
-      <c r="G22" t="s">
+      <c r="I22" t="s">
         <v>72</v>
       </c>
-      <c r="H22" t="s">
+      <c r="J22" t="s">
         <v>73</v>
       </c>
-      <c r="I22" t="s">
-        <v>74</v>
-      </c>
-      <c r="J22" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" ht="12.75" customHeight="1">
+    </row>
+    <row r="23" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>33</v>
       </c>
@@ -1745,26 +1831,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+    <sheetView topLeftCell="A22" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="2" max="2" width="25.1640625" customWidth="1"/>
-    <col min="3" max="3" width="44.1640625" customWidth="1"/>
-    <col min="4" max="1025" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="3" max="3" width="44.140625" customWidth="1"/>
+    <col min="4" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.25" customHeight="1">
+    <row r="1" spans="1:4" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>6</v>
@@ -1773,732 +1859,480 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.25" customHeight="1">
+    <row r="2" spans="1:4" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" t="s">
         <v>78</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>79</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="3" spans="1:4" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" t="s">
         <v>80</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C3" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="16.25" customHeight="1">
-      <c r="A3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>82</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="4" spans="1:4" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" t="s">
         <v>83</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C4" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="16.25" customHeight="1">
-      <c r="A4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>85</v>
       </c>
-      <c r="C4" t="s">
+    </row>
+    <row r="5" spans="1:4" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" t="s">
         <v>86</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C5" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="16.25" customHeight="1">
-      <c r="A5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>88</v>
       </c>
-      <c r="C5" t="s">
+    </row>
+    <row r="6" spans="1:4" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" t="s">
         <v>89</v>
       </c>
-      <c r="D5" t="s">
+      <c r="C6" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="16.25" customHeight="1">
-      <c r="A6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="4" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C8" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="4" customFormat="1" ht="19" customHeight="1">
-      <c r="A8" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C8" s="3" t="s">
+    </row>
+    <row r="9" spans="1:4" s="4" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" s="4" customFormat="1" ht="19" customHeight="1">
-      <c r="A9" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="3" t="s">
+      <c r="D9" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C9" s="3" t="s">
+    </row>
+    <row r="10" spans="1:4" s="4" customFormat="1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" s="4" customFormat="1" ht="16.25" customHeight="1">
-      <c r="A10" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" s="3" t="s">
+      <c r="D10" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C10" s="3" t="s">
+    </row>
+    <row r="11" spans="1:4" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" s="4" customFormat="1" ht="20" customHeight="1">
-      <c r="A11" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="3" t="s">
+      <c r="D11" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C11" s="3" t="s">
+    </row>
+    <row r="12" spans="1:4" s="4" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" s="4" customFormat="1" ht="19" customHeight="1">
-      <c r="A12" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="3" t="s">
+      <c r="D12" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C12" s="3" t="s">
+    </row>
+    <row r="14" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" t="s">
         <v>106</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="18" customHeight="1">
-      <c r="A14" t="s">
-        <v>59</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="D14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" t="s">
         <v>108</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D14" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="16" customHeight="1">
-      <c r="A15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="D15" t="s">
         <v>110</v>
       </c>
-      <c r="C15" s="3" t="s">
+    </row>
+    <row r="16" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" t="s">
         <v>111</v>
       </c>
-      <c r="D15" t="s">
+      <c r="C16" s="3" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="17" customHeight="1">
-      <c r="A16" t="s">
-        <v>59</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="D16" t="s">
         <v>113</v>
       </c>
-      <c r="C16" s="3" t="s">
+    </row>
+    <row r="18" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" t="s">
         <v>114</v>
       </c>
-      <c r="D16" t="s">
+      <c r="C18" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="16" customHeight="1">
-      <c r="A18" t="s">
-        <v>65</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="D18" t="s">
         <v>116</v>
       </c>
-      <c r="C18" t="s">
+    </row>
+    <row r="19" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" t="s">
         <v>117</v>
       </c>
-      <c r="D18" t="s">
+      <c r="C19" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="17" customHeight="1">
-      <c r="A19" t="s">
-        <v>65</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="D19" t="s">
         <v>119</v>
       </c>
-      <c r="C19" t="s">
+    </row>
+    <row r="20" spans="1:4" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" t="s">
         <v>120</v>
       </c>
-      <c r="D19" t="s">
+      <c r="C20" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="19" customHeight="1">
-      <c r="A20" t="s">
-        <v>65</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="D20" t="s">
         <v>122</v>
       </c>
-      <c r="C20" t="s">
+    </row>
+    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" t="s">
         <v>123</v>
       </c>
-      <c r="D20" t="s">
+      <c r="C21" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="15" customHeight="1">
-      <c r="A21" t="s">
-        <v>65</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="D21" t="s">
         <v>125</v>
       </c>
-      <c r="C21" t="s">
+    </row>
+    <row r="22" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" t="s">
         <v>126</v>
       </c>
-      <c r="D21" t="s">
+      <c r="C22" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="16" customHeight="1">
-      <c r="A22" t="s">
-        <v>65</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="D22" t="s">
         <v>128</v>
       </c>
-      <c r="C22" t="s">
+    </row>
+    <row r="24" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" t="s">
         <v>129</v>
       </c>
-      <c r="D22" t="s">
+      <c r="C24" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A24" t="s">
-        <v>53</v>
-      </c>
-      <c r="B24" t="s">
+    <row r="25" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" t="s">
         <v>131</v>
       </c>
-      <c r="C24" t="s">
-        <v>55</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="C25" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A25" t="s">
-        <v>53</v>
-      </c>
-      <c r="B25" t="s">
+      <c r="D25" t="s">
         <v>133</v>
       </c>
-      <c r="C25" t="s">
+    </row>
+    <row r="26" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" t="s">
         <v>134</v>
       </c>
-      <c r="D25" t="s">
+      <c r="C26" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A26" t="s">
-        <v>53</v>
-      </c>
-      <c r="B26" t="s">
+      <c r="D26" t="s">
         <v>136</v>
       </c>
-      <c r="C26" t="s">
+    </row>
+    <row r="28" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" t="s">
         <v>137</v>
       </c>
-      <c r="D26" t="s">
+      <c r="C28" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="16" customHeight="1">
-      <c r="A28" t="s">
-        <v>70</v>
-      </c>
-      <c r="B28" t="s">
+      <c r="D28" t="s">
         <v>139</v>
       </c>
-      <c r="C28" t="s">
+    </row>
+    <row r="29" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>68</v>
+      </c>
+      <c r="B29" t="s">
         <v>140</v>
       </c>
-      <c r="D28" t="s">
+      <c r="C29" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="17" customHeight="1">
-      <c r="A29" t="s">
-        <v>70</v>
-      </c>
-      <c r="B29" t="s">
-        <v>142</v>
-      </c>
-      <c r="C29" t="s">
-        <v>143</v>
-      </c>
       <c r="D29" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="17" customHeight="1">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B30" t="s">
+        <v>103</v>
+      </c>
+      <c r="C30" t="s">
+        <v>104</v>
+      </c>
+      <c r="D30" t="s">
         <v>105</v>
       </c>
-      <c r="C30" t="s">
-        <v>106</v>
-      </c>
-      <c r="D30" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="16" customHeight="1">
+    </row>
+    <row r="33" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>25</v>
       </c>
       <c r="B33" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C33" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D33" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="16" customHeight="1">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>25</v>
       </c>
       <c r="B34" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C34" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D34" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>25</v>
       </c>
       <c r="B35" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C35" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D35" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>25</v>
       </c>
       <c r="B36" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C36" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D36" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>25</v>
       </c>
       <c r="B37" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C37" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D37" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>25</v>
       </c>
       <c r="B38" t="s">
+        <v>152</v>
+      </c>
+      <c r="C38" t="s">
+        <v>153</v>
+      </c>
+      <c r="D38" t="s">
         <v>154</v>
       </c>
-      <c r="C38" t="s">
-        <v>155</v>
-      </c>
-      <c r="D38" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" t="s">
-        <v>43</v>
-      </c>
-      <c r="B40">
-        <v>2017</v>
-      </c>
-      <c r="C40">
-        <v>2017</v>
-      </c>
-      <c r="D40">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>43</v>
-      </c>
-      <c r="B41">
-        <v>2016</v>
-      </c>
-      <c r="C41">
-        <v>2016</v>
-      </c>
-      <c r="D41">
-        <v>2016</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
+        <v>228</v>
+      </c>
+      <c r="B41" t="s">
+        <v>126</v>
+      </c>
+      <c r="C41" t="s">
+        <v>127</v>
+      </c>
+      <c r="D41" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>43</v>
-      </c>
-      <c r="B42">
-        <v>2015</v>
-      </c>
-      <c r="C42">
-        <v>2015</v>
-      </c>
-      <c r="D42">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
+        <v>228</v>
+      </c>
+      <c r="B42" t="s">
+        <v>234</v>
+      </c>
+      <c r="C42" t="s">
+        <v>237</v>
+      </c>
+      <c r="D42" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>43</v>
-      </c>
-      <c r="B43">
-        <v>2014</v>
-      </c>
-      <c r="C43">
-        <v>2014</v>
-      </c>
-      <c r="D43">
-        <v>2014</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
+        <v>228</v>
+      </c>
+      <c r="B43" t="s">
+        <v>235</v>
+      </c>
+      <c r="C43" t="s">
+        <v>238</v>
+      </c>
+      <c r="D43" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>43</v>
-      </c>
-      <c r="B44">
-        <v>2013</v>
-      </c>
-      <c r="C44">
-        <v>2013</v>
-      </c>
-      <c r="D44">
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" t="s">
-        <v>43</v>
-      </c>
-      <c r="B45">
-        <v>2012</v>
-      </c>
-      <c r="C45">
-        <v>2012</v>
-      </c>
-      <c r="D45">
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" t="s">
-        <v>43</v>
-      </c>
-      <c r="B46">
-        <v>2011</v>
-      </c>
-      <c r="C46">
-        <v>2011</v>
-      </c>
-      <c r="D46">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" t="s">
-        <v>43</v>
-      </c>
-      <c r="B47">
-        <v>2010</v>
-      </c>
-      <c r="C47">
-        <v>2010</v>
-      </c>
-      <c r="D47">
-        <v>2010</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" t="s">
-        <v>43</v>
-      </c>
-      <c r="B48">
-        <v>2009</v>
-      </c>
-      <c r="C48">
-        <v>2009</v>
-      </c>
-      <c r="D48">
-        <v>2009</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" t="s">
-        <v>43</v>
-      </c>
-      <c r="B49">
-        <v>2008</v>
-      </c>
-      <c r="C49">
-        <v>2008</v>
-      </c>
-      <c r="D49">
-        <v>2008</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" t="s">
-        <v>43</v>
-      </c>
-      <c r="B50">
-        <v>2007</v>
-      </c>
-      <c r="C50">
-        <v>2007</v>
-      </c>
-      <c r="D50">
-        <v>2007</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" t="s">
-        <v>43</v>
-      </c>
-      <c r="B51">
-        <v>2006</v>
-      </c>
-      <c r="C51">
-        <v>2006</v>
-      </c>
-      <c r="D51">
-        <v>2006</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" t="s">
-        <v>43</v>
-      </c>
-      <c r="B52">
-        <v>2005</v>
-      </c>
-      <c r="C52">
-        <v>2005</v>
-      </c>
-      <c r="D52">
-        <v>2005</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" t="s">
-        <v>43</v>
-      </c>
-      <c r="B53">
-        <v>2004</v>
-      </c>
-      <c r="C53">
-        <v>2004</v>
-      </c>
-      <c r="D53">
-        <v>2004</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" t="s">
-        <v>43</v>
-      </c>
-      <c r="B54">
-        <v>2003</v>
-      </c>
-      <c r="C54">
-        <v>2003</v>
-      </c>
-      <c r="D54">
-        <v>2003</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" t="s">
-        <v>43</v>
-      </c>
-      <c r="B55">
-        <v>2002</v>
-      </c>
-      <c r="C55">
-        <v>2002</v>
-      </c>
-      <c r="D55">
-        <v>2002</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" t="s">
-        <v>43</v>
-      </c>
-      <c r="B56">
-        <v>2001</v>
-      </c>
-      <c r="C56">
-        <v>2001</v>
-      </c>
-      <c r="D56">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" t="s">
-        <v>43</v>
-      </c>
-      <c r="B57">
-        <v>2000</v>
-      </c>
-      <c r="C57">
-        <v>2000</v>
-      </c>
-      <c r="D57">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" t="s">
-        <v>230</v>
-      </c>
-      <c r="B59" t="s">
-        <v>128</v>
-      </c>
-      <c r="C59" t="s">
-        <v>129</v>
-      </c>
-      <c r="D59" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="A60" t="s">
-        <v>230</v>
-      </c>
-      <c r="B60" t="s">
+        <v>228</v>
+      </c>
+      <c r="B44" t="s">
         <v>236</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C44" t="s">
         <v>239</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D44" t="s">
         <v>242</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="A61" t="s">
-        <v>230</v>
-      </c>
-      <c r="B61" t="s">
-        <v>237</v>
-      </c>
-      <c r="C61" t="s">
-        <v>240</v>
-      </c>
-      <c r="D61" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="A62" t="s">
-        <v>230</v>
-      </c>
-      <c r="B62" t="s">
-        <v>238</v>
-      </c>
-      <c r="C62" t="s">
-        <v>241</v>
-      </c>
-      <c r="D62" t="s">
-        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -2520,175 +2354,175 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.83203125" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" customWidth="1"/>
-    <col min="4" max="4" width="19.5" customWidth="1"/>
-    <col min="5" max="5" width="17.5" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" customWidth="1"/>
-    <col min="7" max="9" width="39.6640625" customWidth="1"/>
-    <col min="10" max="10" width="39.33203125" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" customWidth="1"/>
+    <col min="7" max="9" width="39.5703125" customWidth="1"/>
+    <col min="10" max="10" width="39.42578125" customWidth="1"/>
     <col min="11" max="11" width="43" customWidth="1"/>
-    <col min="12" max="1025" width="10.83203125" customWidth="1"/>
+    <col min="12" max="1025" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15">
+    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="J1" t="s">
         <v>164</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="K1" t="s">
         <v>165</v>
       </c>
-      <c r="J1" t="s">
-        <v>166</v>
-      </c>
-      <c r="K1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="15">
+    </row>
+    <row r="2" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>31</v>
       </c>
       <c r="B2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" s="10" t="s">
         <v>169</v>
-      </c>
-      <c r="D2" t="s">
-        <v>169</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>170</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>171</v>
       </c>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
       <c r="I2" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="J2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="15">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D3" t="s">
+        <v>172</v>
+      </c>
+      <c r="E3" t="s">
+        <v>173</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>174</v>
-      </c>
-      <c r="D3" t="s">
-        <v>174</v>
-      </c>
-      <c r="E3" t="s">
-        <v>175</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>176</v>
       </c>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
       <c r="I3" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="J3" t="s">
+        <v>171</v>
+      </c>
+      <c r="K3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>176</v>
+      </c>
+      <c r="B4" t="s">
         <v>177</v>
       </c>
-      <c r="J3" t="s">
-        <v>173</v>
-      </c>
-      <c r="K3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="75">
-      <c r="A4" t="s">
+      <c r="G4" t="s">
         <v>178</v>
       </c>
-      <c r="B4" t="s">
+      <c r="H4" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="G4" t="s">
+      <c r="J4" t="s">
+        <v>171</v>
+      </c>
+      <c r="K4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>180</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="B5" t="s">
+        <v>177</v>
+      </c>
+      <c r="G5" t="s">
+        <v>178</v>
+      </c>
+      <c r="H5" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="J4" t="s">
-        <v>173</v>
-      </c>
-      <c r="K4" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="75">
-      <c r="A5" t="s">
+      <c r="J5" t="s">
+        <v>171</v>
+      </c>
+      <c r="K5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>182</v>
       </c>
-      <c r="B5" t="s">
-        <v>179</v>
-      </c>
-      <c r="G5" t="s">
-        <v>180</v>
-      </c>
-      <c r="H5" s="11" t="s">
+      <c r="B6" t="s">
+        <v>177</v>
+      </c>
+      <c r="G6" t="s">
         <v>183</v>
       </c>
-      <c r="J5" t="s">
-        <v>173</v>
-      </c>
-      <c r="K5" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="75">
-      <c r="A6" t="s">
+      <c r="H6" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="B6" t="s">
-        <v>179</v>
-      </c>
-      <c r="G6" t="s">
-        <v>185</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>186</v>
-      </c>
       <c r="J6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -2710,154 +2544,154 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="12" customWidth="1"/>
-    <col min="3" max="3" width="34.5" style="12" customWidth="1"/>
-    <col min="4" max="1025" width="10.83203125" style="12" customWidth="1"/>
+    <col min="1" max="2" width="10.85546875" style="12" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" style="12" customWidth="1"/>
+    <col min="4" max="1025" width="10.85546875" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>187</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>188</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>189</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="12" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="12" t="s">
+      <c r="C2" s="12" t="s">
         <v>191</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="D2" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="E2" s="12" t="s">
         <v>193</v>
       </c>
-      <c r="D2" s="12" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="D3" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="B3" s="12" t="s">
+      <c r="D4" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="E4" s="12" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="D3" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="B4" s="12" t="s">
+      <c r="C5" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="D6" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>197</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="E5" s="13" t="s">
+      <c r="E6" s="13" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
       <c r="E7" s="13"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="E8" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="B8" s="10" t="s">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="D9" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="10" t="s">
+      <c r="E9" s="10" t="s">
         <v>207</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -2879,20 +2713,20 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="28.33203125" customWidth="1"/>
-    <col min="4" max="1025" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" customWidth="1"/>
+    <col min="4" max="1025" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.75" customHeight="1">
+    <row r="1" spans="1:6" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C1" t="s">
         <v>6</v>
@@ -2901,75 +2735,75 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
+        <v>209</v>
+      </c>
+      <c r="F1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B2" s="2" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16.75" customHeight="1">
-      <c r="A2" s="2" t="s">
+    <row r="3" spans="1:6" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>214</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="16.75" customHeight="1">
-      <c r="A3" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="16.75" customHeight="1">
-      <c r="A4" s="2" t="s">
-        <v>216</v>
       </c>
       <c r="B4" s="2">
         <v>20170804</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16.75" customHeight="1">
+    <row r="5" spans="1:6" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D5" t="s">
         <v>217</v>
       </c>
-      <c r="C5" s="3" t="s">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>218</v>
-      </c>
-      <c r="D5" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>220</v>
       </c>
       <c r="B6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>219</v>
+      </c>
+      <c r="E7" t="s">
+        <v>220</v>
+      </c>
+      <c r="F7" t="s">
         <v>221</v>
       </c>
-      <c r="E7" t="s">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>222</v>
       </c>
-      <c r="F7" t="s">
+      <c r="E8" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
+      <c r="F8" t="s">
         <v>224</v>
-      </c>
-      <c r="E8" t="s">
-        <v>225</v>
-      </c>
-      <c r="F8" t="s">
-        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -2991,9 +2825,9 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -3001,20 +2835,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -3030,4 +2864,39 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="34.42578125" customWidth="1"/>
+    <col min="2" max="2" width="42.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="102" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>253</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Change health_facility to health_facilities and change admin_region to admin_region_id for clarity
</commit_message>
<xml_diff>
--- a/app/config/tables/refrigerators/forms/refrigerators/refrigerators.xlsx
+++ b/app/config/tables/refrigerators/forms/refrigerators/refrigerators.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="37940" windowHeight="19700" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="37940" windowHeight="19700" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,6 @@
     <sheet name="calculates" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="140001"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="295">
   <si>
     <t>comments</t>
   </si>
@@ -480,45 +479,6 @@
     <t>{}</t>
   </si>
   <si>
-    <t>health_facility</t>
-  </si>
-  <si>
-    <t>admin_region = ?</t>
-  </si>
-  <si>
-    <t>[data('adminRegion')]</t>
-  </si>
-  <si>
-    <t>'facility_id&gt;='+opendatakit.encodeURIValue(0)</t>
-  </si>
-  <si>
-    <t>regionLevel1_csv</t>
-  </si>
-  <si>
-    <t>csv</t>
-  </si>
-  <si>
-    <t>"regions1-2.csv"</t>
-  </si>
-  <si>
-    <t>_.chain(context).pluck('regionLevel1').uniq().map(function(regionLevel1){ return {name:regionLevel1, label:regionLevel1, data_value:regionLevel1, display:{title: {text:regionLevel1}}}; }).value()</t>
-  </si>
-  <si>
-    <t>regionLevel2_csv</t>
-  </si>
-  <si>
-    <t>_.map(context, function(place){ place.name = place.regionLevel2; place.label = place.regionLevel2; place.data_value = place.name; place.display = {title: {text:place.label}}; return place; })</t>
-  </si>
-  <si>
-    <t>regionLevel3_csv</t>
-  </si>
-  <si>
-    <t>"regions2-3.csv"</t>
-  </si>
-  <si>
-    <t>_.map(context, function(place){ place.name = place.regionLevel3; place.label = place.regionLevel3; place.data_value = place.name; place.display = {title: {text:place.label}}; return place; })</t>
-  </si>
-  <si>
     <t>partition</t>
   </si>
   <si>
@@ -980,6 +940,15 @@
   </si>
   <si>
     <t>No aplica</t>
+  </si>
+  <si>
+    <t>1=1</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>health_facilities</t>
   </si>
 </sst>
 </file>
@@ -1088,7 +1057,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1108,9 +1077,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1538,8 +1504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S47"/>
   <sheetViews>
-    <sheetView topLeftCell="D10" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1594,7 +1560,7 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="M1" t="s">
         <v>11</v>
@@ -1608,14 +1574,14 @@
       <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="15" t="s">
-        <v>212</v>
+      <c r="Q1" s="14" t="s">
+        <v>199</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
@@ -1792,24 +1758,24 @@
       </c>
       <c r="E14" s="3"/>
       <c r="F14" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="G14" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="H14" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="I14" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="J14" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D15" s="3" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" t="s">
@@ -1828,40 +1794,40 @@
         <v>44</v>
       </c>
       <c r="K15" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
       <c r="L15" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="Q15" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="R15" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="S15" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D16" s="17" t="s">
-        <v>283</v>
+      <c r="D16" s="16" t="s">
+        <v>270</v>
       </c>
       <c r="E16" s="3"/>
-      <c r="F16" s="17" t="s">
-        <v>284</v>
-      </c>
-      <c r="G16" s="17" t="s">
-        <v>285</v>
+      <c r="F16" s="16" t="s">
+        <v>271</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>272</v>
       </c>
       <c r="H16" t="s">
-        <v>286</v>
-      </c>
-      <c r="I16" s="17" t="s">
-        <v>287</v>
-      </c>
-      <c r="J16" s="17" t="s">
-        <v>288</v>
+        <v>273</v>
+      </c>
+      <c r="I16" s="16" t="s">
+        <v>274</v>
+      </c>
+      <c r="J16" s="16" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="16" customHeight="1" x14ac:dyDescent="0.25">
@@ -1882,23 +1848,23 @@
       <c r="D19" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="17" t="s">
-        <v>276</v>
+      <c r="E19" s="16" t="s">
+        <v>263</v>
       </c>
       <c r="F19" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="G19" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="H19" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="I19" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="J19" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
     </row>
     <row r="20" spans="2:10" ht="16" customHeight="1" x14ac:dyDescent="0.25">
@@ -1906,7 +1872,7 @@
         <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
@@ -1917,19 +1883,19 @@
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="G21" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
       <c r="H21" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="I21" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="J21" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
     </row>
     <row r="22" spans="2:10" ht="16" customHeight="1" x14ac:dyDescent="0.25">
@@ -1938,19 +1904,19 @@
       </c>
       <c r="E22" s="3"/>
       <c r="F22" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="G22" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="H22" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="I22" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="J22" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
     </row>
     <row r="23" spans="2:10" ht="16" customHeight="1" x14ac:dyDescent="0.25">
@@ -2028,16 +1994,16 @@
         <v>57</v>
       </c>
       <c r="F28" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="G28" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
       <c r="H28" t="s">
         <v>58</v>
       </c>
       <c r="I28" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
       <c r="J28" t="s">
         <v>59</v>
@@ -2071,22 +2037,22 @@
         <v>24</v>
       </c>
       <c r="E30" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="F30" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="G30" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="H30" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="I30" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="J30" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
     </row>
     <row r="31" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2103,8 +2069,8 @@
       <c r="D33" t="s">
         <v>24</v>
       </c>
-      <c r="E33" s="17" t="s">
-        <v>278</v>
+      <c r="E33" s="16" t="s">
+        <v>265</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>66</v>
@@ -2127,7 +2093,7 @@
         <v>16</v>
       </c>
       <c r="C34" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
@@ -2138,19 +2104,19 @@
         <v>57</v>
       </c>
       <c r="F38" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="G38" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="H38" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="I38" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="J38" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
@@ -2176,50 +2142,50 @@
         <v>65</v>
       </c>
       <c r="F42" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="G42" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
       <c r="H42" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
       <c r="I42" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="J42" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
       <c r="C43" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
       <c r="E44" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="F44" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="G44" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="H44" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
       <c r="I44" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c r="J44" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
@@ -2240,19 +2206,19 @@
         <v>65</v>
       </c>
       <c r="F47" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="G47" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
       <c r="H47" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
       <c r="I47" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
       <c r="J47" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -2270,7 +2236,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -2384,14 +2350,14 @@
       <c r="A9" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>274</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>275</v>
+      <c r="B9" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>261</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.25">
@@ -2412,90 +2378,90 @@
       <c r="A12" t="s">
         <v>60</v>
       </c>
-      <c r="B12" s="17" t="s">
-        <v>289</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>290</v>
+      <c r="B12" s="16" t="s">
+        <v>276</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>277</v>
       </c>
       <c r="D12" t="s">
-        <v>291</v>
+        <v>278</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>60</v>
       </c>
-      <c r="B13" s="17" t="s">
-        <v>292</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>293</v>
+      <c r="B13" s="16" t="s">
+        <v>279</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>280</v>
       </c>
       <c r="D13" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>60</v>
       </c>
-      <c r="B14" s="17" t="s">
-        <v>295</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>296</v>
+      <c r="B14" s="16" t="s">
+        <v>282</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>283</v>
       </c>
       <c r="D14" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>60</v>
       </c>
-      <c r="B15" s="17" t="s">
-        <v>298</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>299</v>
+      <c r="B15" s="16" t="s">
+        <v>285</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>286</v>
       </c>
       <c r="D15" t="s">
-        <v>300</v>
+        <v>287</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="17" t="s">
-        <v>301</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>302</v>
+      <c r="B16" s="16" t="s">
+        <v>288</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>289</v>
       </c>
       <c r="D16" t="s">
-        <v>303</v>
+        <v>290</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="16" t="s">
         <v>94</v>
       </c>
       <c r="D17" t="s">
-        <v>304</v>
+        <v>291</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
     </row>
     <row r="20" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -2540,8 +2506,8 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="17" t="s">
-        <v>276</v>
+      <c r="A24" s="16" t="s">
+        <v>263</v>
       </c>
       <c r="B24" t="s">
         <v>104</v>
@@ -2554,8 +2520,8 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="17" t="s">
-        <v>276</v>
+      <c r="A25" s="16" t="s">
+        <v>263</v>
       </c>
       <c r="B25" t="s">
         <v>107</v>
@@ -2568,8 +2534,8 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="17" t="s">
-        <v>276</v>
+      <c r="A26" s="16" t="s">
+        <v>263</v>
       </c>
       <c r="B26" t="s">
         <v>85</v>
@@ -2667,7 +2633,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="B37" t="s">
         <v>93</v>
@@ -2676,59 +2642,59 @@
         <v>94</v>
       </c>
       <c r="D37" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="B38" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="C38" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="D38" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>182</v>
+      </c>
+      <c r="B39" t="s">
+        <v>189</v>
+      </c>
+      <c r="C39" t="s">
+        <v>192</v>
+      </c>
+      <c r="D39" t="s">
         <v>195</v>
-      </c>
-      <c r="B39" t="s">
-        <v>202</v>
-      </c>
-      <c r="C39" t="s">
-        <v>205</v>
-      </c>
-      <c r="D39" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="B40" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="C40" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="D40" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="17" t="s">
+      <c r="A42" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="B42" s="17" t="s">
+      <c r="B42" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="C42" s="17" t="s">
+      <c r="C42" s="16" t="s">
         <v>105</v>
       </c>
       <c r="D42" t="s">
@@ -2736,13 +2702,13 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="17" t="s">
+      <c r="A43" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="B43" s="17" t="s">
-        <v>277</v>
-      </c>
-      <c r="C43" s="17" t="s">
+      <c r="B43" s="16" t="s">
+        <v>264</v>
+      </c>
+      <c r="C43" s="16" t="s">
         <v>108</v>
       </c>
       <c r="D43" t="s">
@@ -2750,13 +2716,13 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="17" t="s">
-        <v>278</v>
-      </c>
-      <c r="B45" s="17" t="s">
+      <c r="A45" s="16" t="s">
+        <v>265</v>
+      </c>
+      <c r="B45" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="C45" s="17" t="s">
+      <c r="C45" s="16" t="s">
         <v>105</v>
       </c>
       <c r="D45" t="s">
@@ -2764,13 +2730,13 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="17" t="s">
-        <v>278</v>
-      </c>
-      <c r="B46" s="17" t="s">
+      <c r="A46" s="16" t="s">
+        <v>265</v>
+      </c>
+      <c r="B46" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="C46" s="17" t="s">
+      <c r="C46" s="16" t="s">
         <v>108</v>
       </c>
       <c r="D46" t="s">
@@ -2778,31 +2744,31 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="17" t="s">
-        <v>278</v>
-      </c>
-      <c r="B47" s="17" t="s">
-        <v>279</v>
-      </c>
-      <c r="C47" s="17" t="s">
+      <c r="A47" s="16" t="s">
+        <v>265</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>266</v>
+      </c>
+      <c r="C47" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="D47" s="17" t="s">
+      <c r="D47" s="16" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="17" t="s">
-        <v>262</v>
-      </c>
-      <c r="B50" s="17" t="s">
-        <v>280</v>
-      </c>
-      <c r="C50" s="17" t="s">
-        <v>281</v>
+      <c r="A50" s="16" t="s">
+        <v>249</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>267</v>
+      </c>
+      <c r="C50" s="16" t="s">
+        <v>268</v>
       </c>
       <c r="D50" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -2818,10 +2784,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2912,86 +2878,24 @@
         <v>133</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>294</v>
       </c>
       <c r="D3" t="s">
-        <v>139</v>
+        <v>294</v>
       </c>
       <c r="E3" t="s">
-        <v>140</v>
+        <v>292</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>141</v>
+        <v>293</v>
       </c>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="4" t="s">
-        <v>142</v>
-      </c>
+      <c r="I3" s="4"/>
       <c r="J3" t="s">
         <v>138</v>
       </c>
       <c r="K3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="77.5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>143</v>
-      </c>
-      <c r="B4" t="s">
-        <v>144</v>
-      </c>
-      <c r="G4" t="s">
-        <v>145</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="J4" t="s">
-        <v>138</v>
-      </c>
-      <c r="K4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="93" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>147</v>
-      </c>
-      <c r="B5" t="s">
-        <v>144</v>
-      </c>
-      <c r="G5" t="s">
-        <v>145</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="J5" t="s">
-        <v>138</v>
-      </c>
-      <c r="K5" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="93" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>149</v>
-      </c>
-      <c r="B6" t="s">
-        <v>144</v>
-      </c>
-      <c r="G6" t="s">
-        <v>150</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="J6" t="s">
-        <v>138</v>
-      </c>
-      <c r="K6" t="s">
         <v>138</v>
       </c>
     </row>
@@ -3016,111 +2920,111 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="10.81640625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="34.453125" style="12" customWidth="1"/>
-    <col min="4" max="1025" width="10.81640625" style="12" customWidth="1"/>
+    <col min="1" max="2" width="10.81640625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="34.453125" style="11" customWidth="1"/>
+    <col min="4" max="1025" width="10.81640625" style="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="D1" s="12" t="s">
+      <c r="A1" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
-        <v>155</v>
+      <c r="E1" s="11" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>160</v>
+      <c r="A2" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>193</v>
+      <c r="A3" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>194</v>
+      <c r="A4" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>166</v>
+        <v>152</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>168</v>
+        <v>146</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -3128,40 +3032,40 @@
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
-      <c r="E7" s="13"/>
+      <c r="E7" s="12"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="B8" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>170</v>
-      </c>
       <c r="D8" s="10" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -3192,11 +3096,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>175</v>
+      <c r="A1" s="13" t="s">
+        <v>162</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="C1" t="s">
         <v>6</v>
@@ -3205,31 +3109,31 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="F1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="B4" s="2">
         <v>20170804</v>
@@ -3237,18 +3141,18 @@
     </row>
     <row r="5" spans="1:6" ht="16.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="D5" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="B6" t="s">
         <v>38</v>
@@ -3256,24 +3160,24 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="E7" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="F7" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="E8" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="F8" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -3307,7 +3211,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="B2" t="s">
         <v>35</v>
@@ -3315,10 +3219,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="B3" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -3352,18 +3256,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="B1" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="100" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>215</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>220</v>
+        <v>202</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add a way to search for model id when creating a new refrigerator
</commit_message>
<xml_diff>
--- a/app/config/tables/refrigerators/forms/refrigerators/refrigerators.xlsx
+++ b/app/config/tables/refrigerators/forms/refrigerators/refrigerators.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="37935" windowHeight="19695" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="37940" windowHeight="19700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="model" sheetId="6" r:id="rId6"/>
     <sheet name="calculates" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="300">
   <si>
     <t>comments</t>
   </si>
@@ -467,15 +467,6 @@
     <t>refrigerator_types</t>
   </si>
   <si>
-    <t>catalog_id &gt;= ?</t>
-  </si>
-  <si>
-    <t>['0']</t>
-  </si>
-  <si>
-    <t>'catalog_id&gt;='+opendatakit.encodeURIValue(0)</t>
-  </si>
-  <si>
     <t>{}</t>
   </si>
   <si>
@@ -946,6 +937,33 @@
   var currYear = currDate.getFullYear();
   return (data('year') &gt;= 1950 &amp;&amp; data('year') &lt;= currYear) || parseInt(data('year')) === -1
 })()</t>
+  </si>
+  <si>
+    <t>model_search_text</t>
+  </si>
+  <si>
+    <t>Model Search</t>
+  </si>
+  <si>
+    <t>Búsqueda de modelo</t>
+  </si>
+  <si>
+    <t>Search for model id:</t>
+  </si>
+  <si>
+    <t>isSessionVariable</t>
+  </si>
+  <si>
+    <t>catalog_id LIKE ? OR model_id LIKE ? OR manufacturer LIKE ?</t>
+  </si>
+  <si>
+    <t>['%' + data('model_search_text') + '%', '%' + data('model_search_text') + '%', '%' + data('model_search_text') + '%']</t>
+  </si>
+  <si>
+    <t>Search by PIS/PQS Code, Model Id, or Manufacturer</t>
+  </si>
+  <si>
+    <t>Buscar por código PIS / PQS, ID de modelo o fabricante</t>
   </si>
 </sst>
 </file>
@@ -1499,30 +1517,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S47"/>
+  <dimension ref="A1:S50"/>
   <sheetViews>
-    <sheetView topLeftCell="B15" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.85546875" customWidth="1"/>
-    <col min="2" max="3" width="11.42578125" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" customWidth="1"/>
-    <col min="6" max="6" width="24.5703125" customWidth="1"/>
-    <col min="7" max="7" width="29.5703125" customWidth="1"/>
-    <col min="8" max="8" width="30.42578125" customWidth="1"/>
-    <col min="9" max="9" width="41.5703125" customWidth="1"/>
-    <col min="10" max="10" width="22.85546875" customWidth="1"/>
-    <col min="11" max="11" width="19.5703125" customWidth="1"/>
-    <col min="12" max="12" width="20.28515625" customWidth="1"/>
-    <col min="13" max="13" width="16.140625" customWidth="1"/>
-    <col min="14" max="1026" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="42.81640625" customWidth="1"/>
+    <col min="2" max="3" width="11.453125" customWidth="1"/>
+    <col min="4" max="4" width="20.453125" customWidth="1"/>
+    <col min="5" max="5" width="25.1796875" customWidth="1"/>
+    <col min="6" max="6" width="24.54296875" customWidth="1"/>
+    <col min="7" max="7" width="29.54296875" customWidth="1"/>
+    <col min="8" max="8" width="30.453125" customWidth="1"/>
+    <col min="9" max="9" width="41.54296875" customWidth="1"/>
+    <col min="10" max="10" width="22.81640625" customWidth="1"/>
+    <col min="11" max="11" width="19.54296875" customWidth="1"/>
+    <col min="12" max="12" width="20.26953125" customWidth="1"/>
+    <col min="13" max="13" width="16.1796875" customWidth="1"/>
+    <col min="14" max="1026" width="11.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1557,7 +1575,7 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="M1" t="s">
         <v>11</v>
@@ -1572,23 +1590,23 @@
         <v>14</v>
       </c>
       <c r="Q1" s="14" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>16</v>
       </c>
@@ -1596,7 +1614,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>18</v>
       </c>
@@ -1622,7 +1640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" t="s">
         <v>23</v>
@@ -1630,7 +1648,7 @@
       <c r="D5" s="3"/>
       <c r="M5" s="6"/>
     </row>
-    <row r="6" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D6" s="3" t="s">
         <v>24</v>
       </c>
@@ -1656,7 +1674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>16</v>
       </c>
@@ -1666,556 +1684,600 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>31</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="E8" s="3"/>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>291</v>
       </c>
       <c r="G8" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="H8" t="s">
-        <v>28</v>
+        <v>293</v>
       </c>
       <c r="I8" t="s">
-        <v>29</v>
-      </c>
-      <c r="J8" t="s">
-        <v>28</v>
+        <v>294</v>
+      </c>
+      <c r="K8" t="s">
+        <v>298</v>
+      </c>
+      <c r="L8" t="s">
+        <v>299</v>
       </c>
       <c r="P8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>23</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>33</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12" t="s">
+        <v>29</v>
+      </c>
+      <c r="J12" t="s">
+        <v>28</v>
+      </c>
+      <c r="P12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="E12" s="3"/>
-      <c r="F12" t="s">
-        <v>35</v>
-      </c>
-      <c r="O12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D13" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="3"/>
-      <c r="F13" t="s">
-        <v>38</v>
-      </c>
-      <c r="G13" t="s">
-        <v>39</v>
-      </c>
-      <c r="H13" t="s">
-        <v>40</v>
-      </c>
-      <c r="I13" t="s">
-        <v>41</v>
-      </c>
-      <c r="J13" t="s">
-        <v>40</v>
-      </c>
-      <c r="P13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D14" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" s="3"/>
-      <c r="F14" t="s">
-        <v>209</v>
-      </c>
-      <c r="G14" t="s">
-        <v>210</v>
-      </c>
-      <c r="H14" t="s">
-        <v>211</v>
-      </c>
-      <c r="I14" t="s">
-        <v>212</v>
-      </c>
-      <c r="J14" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D15" s="3" t="s">
-        <v>197</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" t="s">
+        <v>35</v>
+      </c>
+      <c r="O15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" t="s">
+        <v>39</v>
+      </c>
+      <c r="H16" t="s">
+        <v>40</v>
+      </c>
+      <c r="I16" t="s">
+        <v>41</v>
+      </c>
+      <c r="J16" t="s">
+        <v>40</v>
+      </c>
+      <c r="P16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" t="s">
+        <v>206</v>
+      </c>
+      <c r="G17" t="s">
+        <v>207</v>
+      </c>
+      <c r="H17" t="s">
+        <v>208</v>
+      </c>
+      <c r="I17" t="s">
+        <v>209</v>
+      </c>
+      <c r="J17" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="18" spans="2:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E18" s="3"/>
+      <c r="F18" t="s">
         <v>42</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G18" t="s">
         <v>43</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H18" t="s">
         <v>44</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I18" t="s">
         <v>45</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J18" t="s">
         <v>44</v>
       </c>
-      <c r="K15" t="s">
-        <v>207</v>
-      </c>
-      <c r="L15" t="s">
-        <v>208</v>
-      </c>
-      <c r="Q15" t="s">
+      <c r="K18" t="s">
+        <v>204</v>
+      </c>
+      <c r="L18" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>199</v>
+      </c>
+      <c r="R18" t="s">
         <v>202</v>
       </c>
-      <c r="R15" t="s">
-        <v>205</v>
-      </c>
-      <c r="S15" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
+      <c r="S18" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="19" spans="2:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="2:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D17" s="16" t="s">
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="2:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D20" s="16" t="s">
+        <v>265</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="16" t="s">
+        <v>266</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>267</v>
+      </c>
+      <c r="H20" t="s">
         <v>268</v>
       </c>
-      <c r="E17" s="3"/>
-      <c r="F17" s="16" t="s">
+      <c r="I20" s="16" t="s">
         <v>269</v>
       </c>
-      <c r="G17" s="16" t="s">
+      <c r="J20" s="16" t="s">
         <v>270</v>
       </c>
-      <c r="H17" t="s">
-        <v>271</v>
-      </c>
-      <c r="I17" s="16" t="s">
-        <v>272</v>
-      </c>
-      <c r="J17" s="16" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
+    </row>
+    <row r="21" spans="2:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="2:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D19" s="3" t="s">
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="2:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D22" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="16" t="s">
-        <v>261</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="E22" s="16" t="s">
+        <v>258</v>
+      </c>
+      <c r="F22" t="s">
+        <v>211</v>
+      </c>
+      <c r="G22" t="s">
+        <v>212</v>
+      </c>
+      <c r="H22" t="s">
         <v>214</v>
       </c>
-      <c r="G19" t="s">
+      <c r="I22" t="s">
+        <v>213</v>
+      </c>
+      <c r="J22" t="s">
         <v>215</v>
       </c>
-      <c r="H19" t="s">
-        <v>217</v>
-      </c>
-      <c r="I19" t="s">
+    </row>
+    <row r="23" spans="2:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" t="s">
         <v>216</v>
-      </c>
-      <c r="J19" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" t="s">
-        <v>219</v>
-      </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="2:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D21" t="s">
-        <v>37</v>
-      </c>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="G21" t="s">
-        <v>222</v>
-      </c>
-      <c r="H21" t="s">
-        <v>223</v>
-      </c>
-      <c r="I21" t="s">
-        <v>224</v>
-      </c>
-      <c r="J21" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D22" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E22" s="3"/>
-      <c r="F22" t="s">
-        <v>221</v>
-      </c>
-      <c r="G22" t="s">
-        <v>226</v>
-      </c>
-      <c r="H22" t="s">
-        <v>227</v>
-      </c>
-      <c r="I22" t="s">
-        <v>228</v>
-      </c>
-      <c r="J22" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" t="s">
-        <v>23</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="2:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
+    <row r="24" spans="2:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="G24" t="s">
+        <v>219</v>
+      </c>
+      <c r="H24" t="s">
+        <v>220</v>
+      </c>
+      <c r="I24" t="s">
+        <v>221</v>
+      </c>
+      <c r="J24" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="25" spans="2:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D25" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" s="3"/>
+      <c r="F25" t="s">
+        <v>218</v>
+      </c>
+      <c r="G25" t="s">
+        <v>223</v>
+      </c>
+      <c r="H25" t="s">
+        <v>224</v>
+      </c>
+      <c r="I25" t="s">
+        <v>225</v>
+      </c>
+      <c r="J25" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="26" spans="2:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="2:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
         <v>33</v>
       </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-    </row>
-    <row r="25" spans="2:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="2:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-    </row>
-    <row r="26" spans="2:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D26" t="s">
-        <v>24</v>
-      </c>
-      <c r="E26" t="s">
-        <v>46</v>
-      </c>
-      <c r="F26" t="s">
-        <v>47</v>
-      </c>
-      <c r="G26" t="s">
-        <v>48</v>
-      </c>
-      <c r="H26" t="s">
-        <v>49</v>
-      </c>
-      <c r="I26" t="s">
-        <v>50</v>
-      </c>
-      <c r="J26" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D27" t="s">
-        <v>24</v>
-      </c>
-      <c r="E27" t="s">
-        <v>51</v>
-      </c>
-      <c r="F27" t="s">
-        <v>52</v>
-      </c>
-      <c r="G27" t="s">
-        <v>53</v>
-      </c>
-      <c r="H27" t="s">
-        <v>54</v>
-      </c>
-      <c r="I27" t="s">
-        <v>55</v>
-      </c>
-      <c r="J27" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D28" t="s">
-        <v>24</v>
-      </c>
-      <c r="E28" t="s">
-        <v>57</v>
-      </c>
-      <c r="F28" t="s">
-        <v>232</v>
-      </c>
-      <c r="G28" t="s">
-        <v>230</v>
-      </c>
-      <c r="H28" t="s">
-        <v>58</v>
-      </c>
-      <c r="I28" t="s">
-        <v>231</v>
-      </c>
-      <c r="J28" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="2:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
         <v>24</v>
       </c>
       <c r="E29" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="F29" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="G29" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="H29" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="I29" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="J29" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
         <v>24</v>
       </c>
       <c r="E30" t="s">
-        <v>181</v>
+        <v>51</v>
       </c>
       <c r="F30" t="s">
-        <v>182</v>
+        <v>52</v>
       </c>
       <c r="G30" t="s">
-        <v>183</v>
+        <v>53</v>
       </c>
       <c r="H30" t="s">
-        <v>184</v>
+        <v>54</v>
       </c>
       <c r="I30" t="s">
-        <v>185</v>
+        <v>55</v>
       </c>
       <c r="J30" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="2:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>24</v>
+      </c>
+      <c r="E31" t="s">
+        <v>57</v>
+      </c>
+      <c r="F31" t="s">
+        <v>229</v>
+      </c>
+      <c r="G31" t="s">
+        <v>227</v>
+      </c>
+      <c r="H31" t="s">
+        <v>58</v>
+      </c>
+      <c r="I31" t="s">
+        <v>228</v>
+      </c>
+      <c r="J31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>24</v>
+      </c>
+      <c r="E32" t="s">
+        <v>60</v>
+      </c>
+      <c r="F32" t="s">
+        <v>61</v>
+      </c>
+      <c r="G32" t="s">
+        <v>62</v>
+      </c>
+      <c r="H32" t="s">
+        <v>63</v>
+      </c>
+      <c r="I32" t="s">
+        <v>64</v>
+      </c>
+      <c r="J32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
         <v>24</v>
       </c>
-      <c r="E33" s="16" t="s">
-        <v>263</v>
-      </c>
-      <c r="F33" s="3" t="s">
+      <c r="E33" t="s">
+        <v>178</v>
+      </c>
+      <c r="F33" t="s">
+        <v>179</v>
+      </c>
+      <c r="G33" t="s">
+        <v>180</v>
+      </c>
+      <c r="H33" t="s">
+        <v>181</v>
+      </c>
+      <c r="I33" t="s">
+        <v>182</v>
+      </c>
+      <c r="J33" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>24</v>
+      </c>
+      <c r="E36" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="F36" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="G33" t="s">
+      <c r="G36" t="s">
         <v>67</v>
       </c>
-      <c r="H33" t="s">
+      <c r="H36" t="s">
         <v>68</v>
       </c>
-      <c r="I33" t="s">
+      <c r="I36" t="s">
         <v>69</v>
       </c>
-      <c r="J33" t="s">
+      <c r="J36" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B34" t="s">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
         <v>16</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C37" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>24</v>
+      </c>
+      <c r="E41" t="s">
+        <v>57</v>
+      </c>
+      <c r="F41" t="s">
+        <v>232</v>
+      </c>
+      <c r="G41" t="s">
+        <v>231</v>
+      </c>
+      <c r="H41" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="D38" t="s">
+      <c r="I41" t="s">
+        <v>234</v>
+      </c>
+      <c r="J41" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
         <v>24</v>
       </c>
-      <c r="E38" t="s">
-        <v>57</v>
-      </c>
-      <c r="F38" t="s">
-        <v>235</v>
-      </c>
-      <c r="G38" t="s">
-        <v>234</v>
-      </c>
-      <c r="H38" t="s">
+      <c r="E45" t="s">
+        <v>65</v>
+      </c>
+      <c r="F45" t="s">
         <v>236</v>
       </c>
-      <c r="I38" t="s">
+      <c r="G45" t="s">
         <v>237</v>
       </c>
-      <c r="J38" t="s">
+      <c r="H45" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B39" t="s">
+      <c r="I45" t="s">
+        <v>239</v>
+      </c>
+      <c r="J45" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>241</v>
+      </c>
+      <c r="C46" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>243</v>
+      </c>
+      <c r="E47" t="s">
+        <v>244</v>
+      </c>
+      <c r="F47" t="s">
+        <v>245</v>
+      </c>
+      <c r="G47" t="s">
+        <v>246</v>
+      </c>
+      <c r="H47" t="s">
+        <v>247</v>
+      </c>
+      <c r="I47" t="s">
+        <v>248</v>
+      </c>
+      <c r="J47" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B40" t="s">
+    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B41" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="D42" t="s">
+    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
         <v>24</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E50" t="s">
         <v>65</v>
       </c>
-      <c r="F42" t="s">
-        <v>239</v>
-      </c>
-      <c r="G42" t="s">
-        <v>240</v>
-      </c>
-      <c r="H42" t="s">
-        <v>241</v>
-      </c>
-      <c r="I42" t="s">
-        <v>242</v>
-      </c>
-      <c r="J42" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B43" t="s">
-        <v>244</v>
-      </c>
-      <c r="C43" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="D44" t="s">
-        <v>246</v>
-      </c>
-      <c r="E44" t="s">
-        <v>247</v>
-      </c>
-      <c r="F44" t="s">
-        <v>248</v>
-      </c>
-      <c r="G44" t="s">
-        <v>249</v>
-      </c>
-      <c r="H44" t="s">
+      <c r="F50" t="s">
         <v>250</v>
       </c>
-      <c r="I44" t="s">
+      <c r="G50" t="s">
         <v>251</v>
       </c>
-      <c r="J44" t="s">
+      <c r="H50" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B45" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B46" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="D47" t="s">
-        <v>24</v>
-      </c>
-      <c r="E47" t="s">
-        <v>65</v>
-      </c>
-      <c r="F47" t="s">
+      <c r="I50" t="s">
         <v>253</v>
       </c>
-      <c r="G47" t="s">
+      <c r="J50" t="s">
         <v>254</v>
-      </c>
-      <c r="H47" t="s">
-        <v>255</v>
-      </c>
-      <c r="I47" t="s">
-        <v>256</v>
-      </c>
-      <c r="J47" t="s">
-        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -2237,15 +2299,15 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" customWidth="1"/>
-    <col min="3" max="3" width="44.140625" customWidth="1"/>
-    <col min="4" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.54296875" customWidth="1"/>
+    <col min="2" max="2" width="25.1796875" customWidth="1"/>
+    <col min="3" max="3" width="44.1796875" customWidth="1"/>
+    <col min="4" max="1025" width="8.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>71</v>
       </c>
@@ -2259,7 +2321,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="4" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" s="4" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>46</v>
       </c>
@@ -2273,7 +2335,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="4" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" s="4" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>46</v>
       </c>
@@ -2287,7 +2349,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="4" customFormat="1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" s="4" customFormat="1" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>46</v>
       </c>
@@ -2301,7 +2363,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" s="4" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>46</v>
       </c>
@@ -2315,7 +2377,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="4" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" s="4" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>46</v>
       </c>
@@ -2329,7 +2391,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>57</v>
       </c>
@@ -2343,21 +2405,21 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>57</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>60</v>
       </c>
@@ -2371,77 +2433,77 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>60</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D12" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>60</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D13" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>60</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D14" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>60</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D15" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>60</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D16" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>60</v>
       </c>
@@ -2452,15 +2514,15 @@
         <v>94</v>
       </c>
       <c r="D17" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16"/>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
     </row>
-    <row r="20" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>51</v>
       </c>
@@ -2474,7 +2536,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -2488,7 +2550,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -2502,9 +2564,9 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B24" t="s">
         <v>104</v>
@@ -2516,9 +2578,9 @@
         <v>106</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B25" t="s">
         <v>107</v>
@@ -2530,9 +2592,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B26" t="s">
         <v>85</v>
@@ -2544,7 +2606,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>25</v>
       </c>
@@ -2558,7 +2620,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>25</v>
       </c>
@@ -2572,7 +2634,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>25</v>
       </c>
@@ -2586,7 +2648,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>25</v>
       </c>
@@ -2600,7 +2662,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>25</v>
       </c>
@@ -2614,7 +2676,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>25</v>
       </c>
@@ -2628,9 +2690,9 @@
         <v>121</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B37" t="s">
         <v>93</v>
@@ -2639,52 +2701,52 @@
         <v>94</v>
       </c>
       <c r="D37" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B38" t="s">
+        <v>184</v>
+      </c>
+      <c r="C38" t="s">
         <v>187</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>190</v>
       </c>
-      <c r="D38" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B39" t="s">
+        <v>185</v>
+      </c>
+      <c r="C39" t="s">
         <v>188</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>191</v>
       </c>
-      <c r="D39" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B40" t="s">
+        <v>186</v>
+      </c>
+      <c r="C40" t="s">
         <v>189</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>192</v>
       </c>
-      <c r="D40" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
         <v>65</v>
       </c>
@@ -2698,12 +2760,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
         <v>65</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C43" s="16" t="s">
         <v>108</v>
@@ -2712,9 +2774,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B45" s="16" t="s">
         <v>104</v>
@@ -2726,9 +2788,9 @@
         <v>106</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="16" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B46" s="16" t="s">
         <v>107</v>
@@ -2740,12 +2802,12 @@
         <v>108</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C47" s="16" t="s">
         <v>95</v>
@@ -2754,18 +2816,18 @@
         <v>95</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="16" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C50" s="16" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D50" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -2783,25 +2845,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" customWidth="1"/>
-    <col min="7" max="9" width="39.5703125" customWidth="1"/>
-    <col min="10" max="10" width="39.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.81640625" customWidth="1"/>
+    <col min="2" max="2" width="21.453125" customWidth="1"/>
+    <col min="3" max="3" width="17.81640625" customWidth="1"/>
+    <col min="4" max="4" width="19.453125" customWidth="1"/>
+    <col min="5" max="5" width="17.453125" customWidth="1"/>
+    <col min="6" max="6" width="19.453125" customWidth="1"/>
+    <col min="7" max="9" width="39.54296875" customWidth="1"/>
+    <col min="10" max="10" width="39.453125" customWidth="1"/>
     <col min="11" max="11" width="43" customWidth="1"/>
-    <col min="12" max="1025" width="10.85546875" customWidth="1"/>
+    <col min="12" max="1025" width="10.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>122</v>
       </c>
@@ -2836,7 +2898,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>31</v>
       </c>
@@ -2850,24 +2912,22 @@
         <v>134</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>135</v>
+        <v>296</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>136</v>
+        <v>297</v>
       </c>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
-      <c r="I2" s="4" t="s">
-        <v>137</v>
-      </c>
+      <c r="I2" s="4"/>
       <c r="J2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="K2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -2875,25 +2935,25 @@
         <v>133</v>
       </c>
       <c r="C3" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D3" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="E3" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
       <c r="I3" s="4"/>
       <c r="J3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="K3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -2915,154 +2975,154 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="10.85546875" style="11" customWidth="1"/>
-    <col min="3" max="3" width="34.42578125" style="11" customWidth="1"/>
-    <col min="4" max="1025" width="10.85546875" style="11" customWidth="1"/>
+    <col min="1" max="2" width="10.81640625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="34.453125" style="11" customWidth="1"/>
+    <col min="4" max="1025" width="10.81640625" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="D2" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="E2" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="C2" s="11" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D3" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="D4" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="C5" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D6" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="D5" s="10" t="s">
+      <c r="E6" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
       <c r="E7" s="12"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="C8" s="10" t="s">
+      <c r="B9" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="E8" s="10" t="s">
+      <c r="D9" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="E9" s="10" t="s">
         <v>158</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -3084,20 +3144,20 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" customWidth="1"/>
-    <col min="4" max="1025" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="28.453125" customWidth="1"/>
+    <col min="4" max="1025" width="11.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="16.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C1" t="s">
         <v>6</v>
@@ -3106,75 +3166,75 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="3" spans="1:6" ht="16.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="B3" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>165</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>168</v>
       </c>
       <c r="B4" s="2">
         <v>20170804</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="16.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>169</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="D5" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>172</v>
       </c>
       <c r="B6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>170</v>
+      </c>
+      <c r="E7" t="s">
+        <v>171</v>
+      </c>
+      <c r="F7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>173</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" t="s">
         <v>174</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F8" t="s">
         <v>175</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>176</v>
-      </c>
-      <c r="E8" t="s">
-        <v>177</v>
-      </c>
-      <c r="F8" t="s">
-        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -3190,28 +3250,45 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="33.36328125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B2" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B3" t="s">
+        <v>291</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3237,26 +3314,26 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" customWidth="1"/>
-    <col min="2" max="2" width="42.85546875" customWidth="1"/>
+    <col min="1" max="1" width="34.453125" customWidth="1"/>
+    <col min="2" max="2" width="42.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="102" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="100" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Account for PK data
</commit_message>
<xml_diff>
--- a/app/config/tables/refrigerators/forms/refrigerators/refrigerators.xlsx
+++ b/app/config/tables/refrigerators/forms/refrigerators/refrigerators.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="37935" windowHeight="19695" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="37935" windowHeight="19695" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -957,9 +957,6 @@
     <t>No Instalado</t>
   </si>
   <si>
-    <t>data('model_other')</t>
-  </si>
-  <si>
     <t>catalog_id LIKE ? OR model_id LIKE ? OR manufacturer LIKE ? OR _id = ?</t>
   </si>
   <si>
@@ -967,6 +964,9 @@
   </si>
   <si>
     <t>['%' + data('model_search_text') + '%', '%' + data('model_search_text') + '%', '%' + data('model_search_text') + '%',  data('model_search_text')]</t>
+  </si>
+  <si>
+    <t>data('model_row_id')</t>
   </si>
 </sst>
 </file>
@@ -1522,8 +1522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S53"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1682,7 +1682,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -1696,7 +1696,7 @@
         <v>287</v>
       </c>
       <c r="O8" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -1723,7 +1723,7 @@
         <v>293</v>
       </c>
       <c r="P9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -1745,7 +1745,7 @@
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -1780,7 +1780,7 @@
         <v>28</v>
       </c>
       <c r="P14" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -2874,7 +2874,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -2941,10 +2941,10 @@
         <v>130</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>

</xml_diff>

<commit_message>
Change contact to contact phone number, removed solar harvesting question, removed model question if new refrigerator, added voltage serial number
</commit_message>
<xml_diff>
--- a/app/config/tables/refrigerators/forms/refrigerators/refrigerators.xlsx
+++ b/app/config/tables/refrigerators/forms/refrigerators/refrigerators.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="410">
   <si>
     <t>comments</t>
   </si>
@@ -646,18 +646,6 @@
     <t>Ingrese el nombre del proveedor de servicios de garantía</t>
   </si>
   <si>
-    <t>Warranty Service Provider Contact</t>
-  </si>
-  <si>
-    <t>Contacto del proveedor de servicios de garantía</t>
-  </si>
-  <si>
-    <t>Enter warranty service provider contact:</t>
-  </si>
-  <si>
-    <t>Ingrese al contacto del proveedor de servicios de garantía</t>
-  </si>
-  <si>
     <t>Functional Status</t>
   </si>
   <si>
@@ -724,21 +712,6 @@
     <t>¿Qué tipo de dispositivo de monitoreo de temperatura está en uso?</t>
   </si>
   <si>
-    <t>solar_energy_harvesting</t>
-  </si>
-  <si>
-    <t>Solar Energy Harvesting</t>
-  </si>
-  <si>
-    <t>Cosecha de energía solar</t>
-  </si>
-  <si>
-    <t>Is solar harvesting used?</t>
-  </si>
-  <si>
-    <t>¿Se utiliza la cosecha solar?</t>
-  </si>
-  <si>
     <t>yes_no_unknown</t>
   </si>
   <si>
@@ -895,9 +868,6 @@
     <t>Type de dispositif de contrôle de la température</t>
   </si>
   <si>
-    <t>Récupération de l'énergie solaire</t>
-  </si>
-  <si>
     <t>display.prompt.text.fr</t>
   </si>
   <si>
@@ -947,9 +917,6 @@
   </si>
   <si>
     <t>Quel est le type de dispositif de contrôle de la température utilisé ?</t>
-  </si>
-  <si>
-    <t>L'énergie solaire est-elle récupérée ?</t>
   </si>
   <si>
     <t>Électricité</t>
@@ -1194,9 +1161,6 @@
     <t>¿Funciona el dispositivo de monitoreo de temperatura?</t>
   </si>
   <si>
-    <t>data('solar_energy_harvesting') === 'yes'</t>
-  </si>
-  <si>
     <t>functioning</t>
   </si>
   <si>
@@ -1270,6 +1234,36 @@
   </si>
   <si>
     <t>Falta de poder/combustible</t>
+  </si>
+  <si>
+    <t>Warranty Service Provider Contact Phone Number</t>
+  </si>
+  <si>
+    <t>Número de teléfono de contacto del proveedor de servicios de garantía</t>
+  </si>
+  <si>
+    <t>Enter warranty service provider contact phone number:</t>
+  </si>
+  <si>
+    <t>Ingrese el número de teléfono de contacto del proveedor de servicios de garantía:</t>
+  </si>
+  <si>
+    <t>data('model_row_id') !== null &amp;&amp; data('model_row_id') !== undefined</t>
+  </si>
+  <si>
+    <t>voltage_regulator_serial_number</t>
+  </si>
+  <si>
+    <t>Voltage Regulator Serial Number</t>
+  </si>
+  <si>
+    <t>Número de serie del regulador de voltaje</t>
+  </si>
+  <si>
+    <t>Voltage regulator serial number?</t>
+  </si>
+  <si>
+    <t>¿Número de serie del regulador de voltaje?</t>
   </si>
 </sst>
 </file>
@@ -1394,7 +1388,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1478,6 +1472,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="9"/>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -1917,7 +1914,7 @@
         <v>3</v>
       </c>
       <c r="C1" s="49" t="s">
-        <v>402</v>
+        <v>390</v>
       </c>
       <c r="D1" s="49" t="s">
         <v>0</v>
@@ -1925,19 +1922,19 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="49" t="s">
-        <v>403</v>
+        <v>391</v>
       </c>
       <c r="B2" s="49"/>
       <c r="C2" s="49"/>
     </row>
     <row r="3" spans="1:4" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A3" s="49" t="s">
-        <v>404</v>
+        <v>392</v>
       </c>
       <c r="B3" s="49"/>
       <c r="C3" s="49"/>
       <c r="D3" s="49" t="s">
-        <v>405</v>
+        <v>393</v>
       </c>
     </row>
   </sheetData>
@@ -1950,8 +1947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1997,7 +1994,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>8</v>
@@ -2006,7 +2003,7 @@
         <v>9</v>
       </c>
       <c r="L1" s="27" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="M1" t="s">
         <v>10</v>
@@ -2052,7 +2049,7 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -2061,7 +2058,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="27"/>
       <c r="R3" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="T3" s="14"/>
       <c r="U3" s="3"/>
@@ -2094,7 +2091,7 @@
         <v>22</v>
       </c>
       <c r="I5" s="18" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="J5" t="s">
         <v>21</v>
@@ -2103,7 +2100,7 @@
         <v>22</v>
       </c>
       <c r="L5" s="26" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="S5">
         <v>1</v>
@@ -2119,497 +2116,499 @@
       <c r="L6" s="23"/>
       <c r="P6" s="6"/>
     </row>
-    <row r="7" spans="1:22" s="41" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D7" s="3" t="s">
+    <row r="7" spans="1:22" s="41" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="41" t="s">
+        <v>404</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="P7" s="6"/>
+    </row>
+    <row r="8" spans="1:22" s="41" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="41" t="s">
+      <c r="F8" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="41" t="s">
+      <c r="G8" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="41" t="s">
+      <c r="H8" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="42" t="s">
-        <v>273</v>
-      </c>
-      <c r="J7" s="41" t="s">
+      <c r="I8" s="42" t="s">
+        <v>264</v>
+      </c>
+      <c r="J8" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="K7" s="41" t="s">
+      <c r="K8" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="L7" s="42" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" s="43" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="51"/>
-      <c r="D8" s="44" t="s">
+      <c r="L8" s="42" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" s="41" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="I9" s="42"/>
+      <c r="L9" s="42"/>
+    </row>
+    <row r="10" spans="1:22" s="43" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="51"/>
+      <c r="D10" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="43" t="s">
+      <c r="E10" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="F8" s="43" t="s">
+      <c r="F10" s="43" t="s">
+        <v>383</v>
+      </c>
+      <c r="G10" s="43" t="s">
+        <v>384</v>
+      </c>
+      <c r="H10" s="43" t="s">
+        <v>394</v>
+      </c>
+      <c r="J10" s="43" t="s">
+        <v>385</v>
+      </c>
+      <c r="K10" s="43" t="s">
         <v>395</v>
       </c>
-      <c r="G8" s="43" t="s">
+      <c r="P10" s="52"/>
+    </row>
+    <row r="11" spans="1:22" s="41" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="41" t="s">
+        <v>386</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="P11" s="6"/>
+    </row>
+    <row r="12" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" t="s">
+        <v>252</v>
+      </c>
+      <c r="G12" t="s">
+        <v>253</v>
+      </c>
+      <c r="H12" t="s">
+        <v>254</v>
+      </c>
+      <c r="I12" s="18"/>
+      <c r="J12" t="s">
+        <v>255</v>
+      </c>
+      <c r="L12" s="23"/>
+      <c r="M12" t="s">
+        <v>257</v>
+      </c>
+      <c r="N12" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" s="43" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="44" t="s">
+        <v>388</v>
+      </c>
+      <c r="E13" s="44"/>
+      <c r="J13" s="43" t="s">
+        <v>389</v>
+      </c>
+      <c r="K13" s="43" t="s">
         <v>396</v>
       </c>
-      <c r="H8" s="43" t="s">
-        <v>406</v>
-      </c>
-      <c r="J8" s="43" t="s">
-        <v>397</v>
-      </c>
-      <c r="K8" s="43" t="s">
-        <v>407</v>
-      </c>
-      <c r="P8" s="52"/>
-    </row>
-    <row r="9" spans="1:22" s="41" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="41" t="s">
-        <v>398</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="P9" s="6"/>
-    </row>
-    <row r="10" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D10" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="3"/>
-      <c r="F10" t="s">
-        <v>261</v>
-      </c>
-      <c r="G10" t="s">
-        <v>262</v>
-      </c>
-      <c r="H10" t="s">
-        <v>263</v>
-      </c>
-      <c r="I10" s="18"/>
-      <c r="J10" t="s">
-        <v>264</v>
-      </c>
-      <c r="L10" s="23"/>
-      <c r="M10" t="s">
-        <v>266</v>
-      </c>
-      <c r="N10" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" s="43" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="44" t="s">
-        <v>400</v>
-      </c>
-      <c r="E11" s="44"/>
-      <c r="J11" s="43" t="s">
-        <v>401</v>
-      </c>
-      <c r="K11" s="43" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="41" t="s">
+    </row>
+    <row r="14" spans="1:22" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="41" t="s">
         <v>23</v>
-      </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="I12" s="42"/>
-    </row>
-    <row r="13" spans="1:22" s="41" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="41" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="P13" s="6"/>
-    </row>
-    <row r="14" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" t="s">
-        <v>398</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
-      <c r="I14" s="17"/>
-      <c r="L14" s="23"/>
+      <c r="I14" s="42"/>
     </row>
     <row r="15" spans="1:22" s="41" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="41" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="D15" s="3"/>
       <c r="P15" s="6"/>
     </row>
-    <row r="16" spans="1:22" s="41" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D16" s="3" t="s">
+    <row r="16" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" t="s">
+        <v>386</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="I16" s="17"/>
+      <c r="L16" s="23"/>
+    </row>
+    <row r="17" spans="1:22" s="41" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="P17" s="6"/>
+    </row>
+    <row r="18" spans="1:22" s="41" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="41" t="s">
+      <c r="F18" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="G16" s="41" t="s">
+      <c r="G18" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="H16" s="41" t="s">
+      <c r="H18" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="I16" s="42" t="s">
-        <v>273</v>
-      </c>
-      <c r="J16" s="41" t="s">
+      <c r="I18" s="42" t="s">
+        <v>264</v>
+      </c>
+      <c r="J18" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="K16" s="41" t="s">
+      <c r="K18" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="L16" s="42" t="s">
-        <v>291</v>
-      </c>
-      <c r="S16" s="41" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="17" spans="2:22" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+      <c r="L18" s="42" t="s">
+        <v>281</v>
+      </c>
+      <c r="S18" s="41" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>30</v>
-      </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="I17" s="17"/>
-      <c r="L17" s="23"/>
-    </row>
-    <row r="18" spans="2:22" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="I18" s="17"/>
-      <c r="L18" s="23"/>
-    </row>
-    <row r="19" spans="2:22" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>15</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
-    </row>
-    <row r="20" spans="2:22" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D20" s="3" t="s">
+      <c r="I19" s="17"/>
+      <c r="L19" s="23"/>
+    </row>
+    <row r="20" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="I20" s="17"/>
+      <c r="L20" s="23"/>
+    </row>
+    <row r="21" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D22" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="3"/>
-      <c r="F20" t="s">
+      <c r="E22" s="3"/>
+      <c r="F22" t="s">
         <v>34</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G22" t="s">
         <v>35</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H22" t="s">
         <v>36</v>
       </c>
-      <c r="I20" s="18" t="s">
-        <v>274</v>
-      </c>
-      <c r="J20" t="s">
+      <c r="I22" s="18" t="s">
+        <v>265</v>
+      </c>
+      <c r="J22" t="s">
         <v>37</v>
       </c>
-      <c r="K20" t="s">
+      <c r="K22" t="s">
         <v>36</v>
       </c>
-      <c r="L20" s="24" t="s">
-        <v>292</v>
-      </c>
-      <c r="S20">
+      <c r="L22" s="24" t="s">
+        <v>282</v>
+      </c>
+      <c r="S22">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:22" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D21" s="3" t="s">
+    <row r="23" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D23" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="E21" s="3"/>
-      <c r="F21" t="s">
-        <v>372</v>
-      </c>
-      <c r="G21" t="s">
+      <c r="E23" s="3"/>
+      <c r="F23" t="s">
+        <v>361</v>
+      </c>
+      <c r="G23" t="s">
         <v>38</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H23" t="s">
         <v>39</v>
       </c>
-      <c r="I21" s="18" t="s">
-        <v>276</v>
-      </c>
-      <c r="J21" t="s">
+      <c r="I23" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="J23" t="s">
         <v>40</v>
       </c>
-      <c r="K21" t="s">
+      <c r="K23" t="s">
         <v>39</v>
       </c>
-      <c r="L21" s="24" t="s">
-        <v>294</v>
-      </c>
-      <c r="M21" t="s">
+      <c r="L23" s="24" t="s">
+        <v>284</v>
+      </c>
+      <c r="M23" t="s">
         <v>187</v>
       </c>
-      <c r="N21" t="s">
+      <c r="N23" t="s">
         <v>188</v>
       </c>
-      <c r="T21" t="s">
-        <v>378</v>
-      </c>
-      <c r="U21" t="s">
+      <c r="T23" t="s">
+        <v>367</v>
+      </c>
+      <c r="U23" t="s">
         <v>185</v>
       </c>
-      <c r="V21" t="s">
+      <c r="V23" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="22" spans="2:22" s="43" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D22" s="44" t="s">
+    <row r="24" spans="1:22" s="43" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D24" s="44" t="s">
         <v>179</v>
       </c>
-      <c r="E22" s="44"/>
-      <c r="F22" s="43" t="s">
-        <v>373</v>
-      </c>
-      <c r="G22" s="43" t="s">
-        <v>336</v>
-      </c>
-      <c r="H22" s="43" t="s">
-        <v>338</v>
-      </c>
-      <c r="I22" s="43" t="s">
-        <v>339</v>
-      </c>
-      <c r="J22" s="43" t="s">
-        <v>340</v>
-      </c>
-      <c r="K22" s="43" t="s">
-        <v>338</v>
-      </c>
-      <c r="L22" s="43" t="s">
-        <v>341</v>
-      </c>
-      <c r="M22" s="43" t="s">
+      <c r="E24" s="44"/>
+      <c r="F24" s="43" t="s">
+        <v>362</v>
+      </c>
+      <c r="G24" s="43" t="s">
+        <v>325</v>
+      </c>
+      <c r="H24" s="43" t="s">
+        <v>327</v>
+      </c>
+      <c r="I24" s="43" t="s">
+        <v>328</v>
+      </c>
+      <c r="J24" s="43" t="s">
+        <v>329</v>
+      </c>
+      <c r="K24" s="43" t="s">
+        <v>327</v>
+      </c>
+      <c r="L24" s="43" t="s">
+        <v>330</v>
+      </c>
+      <c r="M24" s="43" t="s">
         <v>187</v>
       </c>
-      <c r="N22" s="43" t="s">
+      <c r="N24" s="43" t="s">
         <v>188</v>
       </c>
-      <c r="T22" s="43" t="s">
-        <v>379</v>
-      </c>
-      <c r="U22" s="43" t="s">
+      <c r="T24" s="43" t="s">
+        <v>368</v>
+      </c>
+      <c r="U24" s="43" t="s">
         <v>185</v>
       </c>
-      <c r="V22" s="43" t="s">
+      <c r="V24" s="43" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="23" spans="2:22" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+    <row r="25" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-    </row>
-    <row r="24" spans="2:22" s="43" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D24" s="45" t="s">
-        <v>244</v>
-      </c>
-      <c r="E24" s="44"/>
-      <c r="F24" s="45" t="s">
-        <v>342</v>
-      </c>
-      <c r="G24" s="45" t="s">
-        <v>337</v>
-      </c>
-      <c r="H24" s="45" t="s">
-        <v>343</v>
-      </c>
-      <c r="J24" s="45" t="s">
-        <v>344</v>
-      </c>
-      <c r="K24" s="45" t="s">
-        <v>345</v>
-      </c>
-      <c r="L24" s="45"/>
-    </row>
-    <row r="25" spans="2:22" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="1:22" s="43" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D26" s="45" t="s">
+        <v>235</v>
+      </c>
+      <c r="E26" s="44"/>
+      <c r="F26" s="45" t="s">
+        <v>331</v>
+      </c>
+      <c r="G26" s="45" t="s">
+        <v>326</v>
+      </c>
+      <c r="H26" s="45" t="s">
+        <v>332</v>
+      </c>
+      <c r="J26" s="45" t="s">
+        <v>333</v>
+      </c>
+      <c r="K26" s="45" t="s">
+        <v>334</v>
+      </c>
+      <c r="L26" s="45"/>
+    </row>
+    <row r="27" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D27" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E25" s="3"/>
-      <c r="F25" t="s">
+      <c r="E27" s="3"/>
+      <c r="F27" t="s">
         <v>189</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G27" t="s">
         <v>190</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H27" t="s">
         <v>191</v>
       </c>
-      <c r="I25" s="18" t="s">
-        <v>275</v>
-      </c>
-      <c r="J25" t="s">
+      <c r="I27" s="18" t="s">
+        <v>266</v>
+      </c>
+      <c r="J27" t="s">
         <v>192</v>
       </c>
-      <c r="K25" t="s">
+      <c r="K27" t="s">
         <v>193</v>
       </c>
-      <c r="L25" s="24" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="26" spans="2:22" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+      <c r="L27" s="24" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
         <v>15</v>
-      </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="I26" s="17"/>
-      <c r="L26" s="23"/>
-    </row>
-    <row r="27" spans="2:22" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D27" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E27" s="16" t="s">
-        <v>237</v>
-      </c>
-      <c r="F27" t="s">
-        <v>194</v>
-      </c>
-      <c r="G27" t="s">
-        <v>195</v>
-      </c>
-      <c r="H27" t="s">
-        <v>197</v>
-      </c>
-      <c r="I27" s="18" t="s">
-        <v>277</v>
-      </c>
-      <c r="J27" t="s">
-        <v>196</v>
-      </c>
-      <c r="K27" t="s">
-        <v>198</v>
-      </c>
-      <c r="L27" s="24" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="28" spans="2:22" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>16</v>
-      </c>
-      <c r="C28" t="s">
-        <v>199</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="I28" s="17"/>
       <c r="L28" s="23"/>
     </row>
-    <row r="29" spans="2:22" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" t="s">
+    <row r="29" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D29" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E29" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="F29" t="s">
+        <v>194</v>
+      </c>
+      <c r="G29" t="s">
+        <v>195</v>
+      </c>
+      <c r="H29" t="s">
+        <v>197</v>
+      </c>
+      <c r="I29" s="18" t="s">
+        <v>268</v>
+      </c>
+      <c r="J29" t="s">
+        <v>196</v>
+      </c>
+      <c r="K29" t="s">
+        <v>198</v>
+      </c>
+      <c r="L29" s="24" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" t="s">
+        <v>199</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="I30" s="17"/>
+      <c r="L30" s="23"/>
+    </row>
+    <row r="31" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
         <v>33</v>
       </c>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3" t="s">
+      <c r="E31" s="3"/>
+      <c r="F31" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G31" t="s">
         <v>202</v>
       </c>
-      <c r="H29" t="s">
+      <c r="H31" t="s">
         <v>203</v>
       </c>
-      <c r="I29" s="20" t="s">
-        <v>278</v>
-      </c>
-      <c r="J29" t="s">
+      <c r="I31" s="20" t="s">
+        <v>269</v>
+      </c>
+      <c r="J31" t="s">
         <v>204</v>
       </c>
-      <c r="K29" t="s">
+      <c r="K31" t="s">
         <v>205</v>
       </c>
-      <c r="L29" s="25" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="30" spans="2:22" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="3" t="s">
+      <c r="L31" s="25" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" s="43" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D32" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="E30" s="3"/>
-      <c r="F30" t="s">
+      <c r="E32" s="44"/>
+      <c r="F32" s="43" t="s">
         <v>201</v>
       </c>
-      <c r="G30" t="s">
-        <v>206</v>
-      </c>
-      <c r="H30" t="s">
-        <v>207</v>
-      </c>
-      <c r="I30" s="22" t="s">
-        <v>279</v>
-      </c>
-      <c r="J30" t="s">
-        <v>208</v>
-      </c>
-      <c r="K30" t="s">
-        <v>209</v>
-      </c>
-      <c r="L30" s="28" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="31" spans="2:22" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>23</v>
-      </c>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="I31" s="17"/>
-      <c r="L31" s="23"/>
-    </row>
-    <row r="32" spans="2:22" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>30</v>
-      </c>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="I32" s="17"/>
-      <c r="L32" s="23"/>
+      <c r="G32" s="43" t="s">
+        <v>400</v>
+      </c>
+      <c r="H32" s="43" t="s">
+        <v>401</v>
+      </c>
+      <c r="I32" s="53" t="s">
+        <v>270</v>
+      </c>
+      <c r="J32" s="43" t="s">
+        <v>402</v>
+      </c>
+      <c r="K32" s="43" t="s">
+        <v>403</v>
+      </c>
+      <c r="L32" s="53" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="33" spans="2:12" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
@@ -2617,451 +2616,444 @@
       <c r="L33" s="23"/>
     </row>
     <row r="34" spans="2:12" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D34" t="s">
-        <v>24</v>
-      </c>
-      <c r="E34" t="s">
-        <v>41</v>
-      </c>
-      <c r="F34" t="s">
-        <v>42</v>
-      </c>
-      <c r="G34" t="s">
-        <v>43</v>
-      </c>
-      <c r="H34" t="s">
-        <v>44</v>
-      </c>
-      <c r="I34" s="18" t="s">
-        <v>280</v>
-      </c>
-      <c r="J34" t="s">
-        <v>45</v>
-      </c>
-      <c r="K34" t="s">
-        <v>44</v>
-      </c>
-      <c r="L34" s="24" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="35" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D35" t="s">
-        <v>24</v>
-      </c>
-      <c r="E35" t="s">
-        <v>46</v>
-      </c>
-      <c r="F35" t="s">
-        <v>47</v>
-      </c>
-      <c r="G35" t="s">
-        <v>48</v>
-      </c>
-      <c r="H35" t="s">
-        <v>49</v>
-      </c>
-      <c r="I35" s="18" t="s">
-        <v>281</v>
-      </c>
-      <c r="J35" t="s">
-        <v>50</v>
-      </c>
-      <c r="K35" t="s">
-        <v>51</v>
-      </c>
-      <c r="L35" s="26" t="s">
-        <v>299</v>
-      </c>
+      <c r="B34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="I34" s="17"/>
+      <c r="L34" s="23"/>
+    </row>
+    <row r="35" spans="2:12" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="I35" s="17"/>
+      <c r="L35" s="23"/>
     </row>
     <row r="36" spans="2:12" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
         <v>24</v>
       </c>
       <c r="E36" t="s">
-        <v>394</v>
+        <v>41</v>
       </c>
       <c r="F36" t="s">
-        <v>212</v>
+        <v>42</v>
       </c>
       <c r="G36" t="s">
-        <v>210</v>
+        <v>43</v>
       </c>
       <c r="H36" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="I36" s="18" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="J36" t="s">
-        <v>211</v>
+        <v>45</v>
       </c>
       <c r="K36" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="L36" s="24" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
     </row>
     <row r="37" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D37" s="14" t="s">
-        <v>225</v>
+      <c r="D37" t="s">
+        <v>24</v>
       </c>
       <c r="E37" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="F37" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="G37" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="H37" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="I37" s="18" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="J37" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="K37" t="s">
-        <v>58</v>
-      </c>
-      <c r="L37" s="24" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="38" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="L37" s="26" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
         <v>24</v>
       </c>
       <c r="E38" t="s">
+        <v>382</v>
+      </c>
+      <c r="F38" t="s">
+        <v>208</v>
+      </c>
+      <c r="G38" t="s">
+        <v>206</v>
+      </c>
+      <c r="H38" t="s">
+        <v>53</v>
+      </c>
+      <c r="I38" s="18" t="s">
+        <v>273</v>
+      </c>
+      <c r="J38" t="s">
+        <v>207</v>
+      </c>
+      <c r="K38" t="s">
+        <v>54</v>
+      </c>
+      <c r="L38" s="24" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D39" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="E39" t="s">
+        <v>55</v>
+      </c>
+      <c r="F39" t="s">
+        <v>56</v>
+      </c>
+      <c r="G39" t="s">
+        <v>57</v>
+      </c>
+      <c r="H39" t="s">
+        <v>58</v>
+      </c>
+      <c r="I39" s="18" t="s">
+        <v>274</v>
+      </c>
+      <c r="J39" t="s">
+        <v>59</v>
+      </c>
+      <c r="K39" t="s">
+        <v>58</v>
+      </c>
+      <c r="L39" s="24" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>24</v>
+      </c>
+      <c r="E40" t="s">
         <v>163</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F40" t="s">
         <v>164</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G40" t="s">
         <v>165</v>
       </c>
-      <c r="H38" t="s">
+      <c r="H40" t="s">
         <v>166</v>
       </c>
-      <c r="I38" s="18" t="s">
-        <v>284</v>
-      </c>
-      <c r="J38" t="s">
+      <c r="I40" s="18" t="s">
+        <v>275</v>
+      </c>
+      <c r="J40" t="s">
         <v>167</v>
       </c>
-      <c r="K38" t="s">
+      <c r="K40" t="s">
         <v>168</v>
       </c>
-      <c r="L38" s="28" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="39" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
+      <c r="L40" s="28" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
         <v>30</v>
-      </c>
-      <c r="I39" s="17"/>
-      <c r="L39" s="23"/>
-    </row>
-    <row r="40" spans="2:12" s="41" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="C40" s="41" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>15</v>
       </c>
       <c r="I41" s="17"/>
       <c r="L41" s="23"/>
     </row>
-    <row r="42" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D42" t="s">
-        <v>24</v>
-      </c>
-      <c r="E42" s="16" t="s">
-        <v>239</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G42" t="s">
-        <v>62</v>
-      </c>
-      <c r="H42" t="s">
-        <v>63</v>
-      </c>
-      <c r="I42" s="19" t="s">
-        <v>285</v>
-      </c>
-      <c r="J42" t="s">
-        <v>64</v>
-      </c>
-      <c r="K42" t="s">
-        <v>65</v>
-      </c>
-      <c r="L42" s="26" t="s">
-        <v>303</v>
+    <row r="42" spans="2:12" s="41" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="C42" s="41" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>16</v>
-      </c>
-      <c r="C43" t="s">
-        <v>213</v>
+        <v>15</v>
       </c>
       <c r="I43" s="17"/>
       <c r="L43" s="23"/>
     </row>
-    <row r="44" spans="2:12" ht="25" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
         <v>24</v>
       </c>
-      <c r="E44" t="s">
-        <v>52</v>
-      </c>
-      <c r="F44" t="s">
-        <v>215</v>
+      <c r="E44" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="G44" t="s">
-        <v>214</v>
+        <v>62</v>
       </c>
       <c r="H44" t="s">
-        <v>216</v>
-      </c>
-      <c r="I44" s="22" t="s">
-        <v>286</v>
+        <v>63</v>
+      </c>
+      <c r="I44" s="19" t="s">
+        <v>276</v>
       </c>
       <c r="J44" t="s">
-        <v>217</v>
+        <v>64</v>
       </c>
       <c r="K44" t="s">
-        <v>218</v>
-      </c>
-      <c r="L44" s="29" t="s">
-        <v>304</v>
+        <v>65</v>
+      </c>
+      <c r="L44" s="26" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>23</v>
+        <v>16</v>
+      </c>
+      <c r="C45" t="s">
+        <v>209</v>
       </c>
       <c r="I45" s="17"/>
       <c r="L45" s="23"/>
     </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>30</v>
-      </c>
-      <c r="I46" s="17"/>
-      <c r="L46" s="23"/>
-    </row>
-    <row r="47" spans="2:12" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="41" t="s">
-        <v>23</v>
+    <row r="46" spans="2:12" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D46" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="F46" s="43" t="s">
+        <v>405</v>
+      </c>
+      <c r="G46" s="43" t="s">
+        <v>406</v>
+      </c>
+      <c r="H46" s="43" t="s">
+        <v>407</v>
+      </c>
+      <c r="J46" s="43" t="s">
+        <v>408</v>
+      </c>
+      <c r="K46" s="43" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" ht="25" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>24</v>
+      </c>
+      <c r="E47" t="s">
+        <v>52</v>
+      </c>
+      <c r="F47" t="s">
+        <v>211</v>
+      </c>
+      <c r="G47" t="s">
+        <v>210</v>
+      </c>
+      <c r="H47" t="s">
+        <v>212</v>
+      </c>
+      <c r="I47" s="22" t="s">
+        <v>277</v>
+      </c>
+      <c r="J47" t="s">
+        <v>213</v>
+      </c>
+      <c r="K47" t="s">
+        <v>214</v>
+      </c>
+      <c r="L47" s="29" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="48" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="I48" s="17"/>
       <c r="L48" s="23"/>
     </row>
-    <row r="49" spans="2:12" ht="25" x14ac:dyDescent="0.25">
-      <c r="D49" t="s">
+    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>30</v>
+      </c>
+      <c r="I49" s="17"/>
+      <c r="L49" s="23"/>
+    </row>
+    <row r="50" spans="2:12" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="41" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>15</v>
+      </c>
+      <c r="I51" s="17"/>
+      <c r="L51" s="23"/>
+    </row>
+    <row r="52" spans="2:12" ht="25" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
         <v>24</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E52" t="s">
         <v>60</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F52" t="s">
+        <v>215</v>
+      </c>
+      <c r="G52" t="s">
+        <v>216</v>
+      </c>
+      <c r="H52" t="s">
+        <v>217</v>
+      </c>
+      <c r="I52" s="22" t="s">
+        <v>278</v>
+      </c>
+      <c r="J52" t="s">
+        <v>218</v>
+      </c>
+      <c r="K52" t="s">
         <v>219</v>
       </c>
-      <c r="G49" t="s">
-        <v>220</v>
-      </c>
-      <c r="H49" t="s">
-        <v>221</v>
-      </c>
-      <c r="I49" s="22" t="s">
-        <v>287</v>
-      </c>
-      <c r="J49" t="s">
-        <v>222</v>
-      </c>
-      <c r="K49" t="s">
-        <v>223</v>
-      </c>
-      <c r="L49" s="26" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>224</v>
-      </c>
-      <c r="C50" t="s">
-        <v>380</v>
-      </c>
-      <c r="I50" s="17"/>
-      <c r="L50" s="23"/>
-    </row>
-    <row r="51" spans="2:12" ht="25" x14ac:dyDescent="0.25">
-      <c r="D51" t="s">
-        <v>33</v>
-      </c>
-      <c r="F51" t="s">
-        <v>227</v>
-      </c>
-      <c r="G51" t="s">
-        <v>228</v>
-      </c>
-      <c r="H51" t="s">
-        <v>229</v>
-      </c>
-      <c r="I51" s="22" t="s">
-        <v>288</v>
-      </c>
-      <c r="J51" t="s">
-        <v>230</v>
-      </c>
-      <c r="K51" t="s">
-        <v>231</v>
-      </c>
-      <c r="L51" s="26" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="52" spans="2:12" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D52" s="41" t="s">
-        <v>24</v>
-      </c>
-      <c r="E52" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="F52" s="41" t="s">
-        <v>381</v>
-      </c>
-      <c r="G52" s="41" t="s">
-        <v>382</v>
-      </c>
-      <c r="H52" s="41" t="s">
-        <v>383</v>
-      </c>
-      <c r="I52" s="28"/>
-      <c r="J52" s="41" t="s">
-        <v>384</v>
-      </c>
-      <c r="K52" s="41" t="s">
-        <v>385</v>
-      </c>
-      <c r="L52" s="34"/>
+      <c r="L52" s="26" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="53" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>23</v>
+        <v>220</v>
+      </c>
+      <c r="C53" t="s">
+        <v>369</v>
       </c>
       <c r="I53" s="17"/>
       <c r="L53" s="23"/>
     </row>
-    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
+    <row r="54" spans="2:12" ht="25" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
+        <v>33</v>
+      </c>
+      <c r="F54" t="s">
+        <v>223</v>
+      </c>
+      <c r="G54" t="s">
+        <v>224</v>
+      </c>
+      <c r="H54" t="s">
+        <v>225</v>
+      </c>
+      <c r="I54" s="22" t="s">
+        <v>279</v>
+      </c>
+      <c r="J54" t="s">
+        <v>226</v>
+      </c>
+      <c r="K54" t="s">
+        <v>227</v>
+      </c>
+      <c r="L54" s="26" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="55" spans="2:12" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D55" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="E55" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="F55" s="41" t="s">
+        <v>370</v>
+      </c>
+      <c r="G55" s="41" t="s">
+        <v>371</v>
+      </c>
+      <c r="H55" s="41" t="s">
+        <v>372</v>
+      </c>
+      <c r="I55" s="28"/>
+      <c r="J55" s="41" t="s">
+        <v>373</v>
+      </c>
+      <c r="K55" s="41" t="s">
+        <v>374</v>
+      </c>
+      <c r="L55" s="34"/>
+    </row>
+    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>23</v>
+      </c>
+      <c r="I56" s="17"/>
+      <c r="L56" s="23"/>
+    </row>
+    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
         <v>30</v>
       </c>
-      <c r="I54" s="17"/>
-      <c r="L54" s="23"/>
-    </row>
-    <row r="55" spans="2:12" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="C55" s="41" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="56" spans="2:12" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="41" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D57" t="s">
-        <v>24</v>
-      </c>
-      <c r="E57" t="s">
-        <v>60</v>
-      </c>
-      <c r="F57" t="s">
-        <v>232</v>
-      </c>
-      <c r="G57" t="s">
-        <v>233</v>
-      </c>
-      <c r="H57" t="s">
-        <v>234</v>
-      </c>
-      <c r="I57" s="18" t="s">
-        <v>289</v>
-      </c>
-      <c r="J57" t="s">
-        <v>235</v>
-      </c>
-      <c r="K57" t="s">
-        <v>236</v>
-      </c>
-      <c r="L57" s="26" t="s">
-        <v>307</v>
-      </c>
+      <c r="I57" s="17"/>
+      <c r="L57" s="23"/>
     </row>
     <row r="58" spans="2:12" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B58" s="41" t="s">
         <v>16</v>
       </c>
       <c r="C58" s="41" t="s">
-        <v>386</v>
-      </c>
-      <c r="I58" s="42"/>
-      <c r="L58" s="34"/>
-    </row>
-    <row r="59" spans="2:12" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D59" s="43" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="59" spans="2:12" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="41" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60" spans="2:12" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D60" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="E59" s="43" t="s">
+      <c r="E60" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="F59" s="43" t="s">
-        <v>349</v>
-      </c>
-      <c r="G59" s="43" t="s">
-        <v>350</v>
-      </c>
-      <c r="H59" s="43" t="s">
-        <v>351</v>
-      </c>
-      <c r="J59" s="43" t="s">
-        <v>348</v>
-      </c>
-      <c r="K59" s="43" t="s">
-        <v>352</v>
-      </c>
-      <c r="L59" s="45"/>
-    </row>
-    <row r="60" spans="2:12" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="L60" s="34"/>
+      <c r="F60" s="43" t="s">
+        <v>338</v>
+      </c>
+      <c r="G60" s="43" t="s">
+        <v>339</v>
+      </c>
+      <c r="H60" s="43" t="s">
+        <v>340</v>
+      </c>
+      <c r="J60" s="43" t="s">
+        <v>337</v>
+      </c>
+      <c r="K60" s="43" t="s">
+        <v>341</v>
+      </c>
+      <c r="L60" s="45"/>
     </row>
     <row r="61" spans="2:12" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B61" s="42" t="s">
@@ -3112,7 +3104,7 @@
         <v>7</v>
       </c>
       <c r="E1" s="33" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="4" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -3129,7 +3121,7 @@
         <v>70</v>
       </c>
       <c r="E2" s="32" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="4" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -3146,7 +3138,7 @@
         <v>73</v>
       </c>
       <c r="E3" s="32" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="4" customFormat="1" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -3163,7 +3155,7 @@
         <v>76</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="4" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -3180,7 +3172,7 @@
         <v>79</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="4" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -3197,7 +3189,7 @@
         <v>82</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="4" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -3211,16 +3203,16 @@
         <v>52</v>
       </c>
       <c r="B8" s="41" t="s">
-        <v>387</v>
+        <v>375</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>388</v>
+        <v>376</v>
       </c>
       <c r="D8" s="41" t="s">
         <v>53</v>
       </c>
       <c r="E8" s="38" t="s">
-        <v>389</v>
+        <v>377</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="41" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.25">
@@ -3228,45 +3220,45 @@
         <v>52</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>390</v>
+        <v>378</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>391</v>
+        <v>379</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="E9" s="47" t="s">
-        <v>393</v>
+        <v>381</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="43" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="43" t="s">
-        <v>394</v>
+        <v>382</v>
       </c>
       <c r="B11" s="46" t="s">
-        <v>387</v>
+        <v>375</v>
       </c>
       <c r="C11" s="46" t="s">
-        <v>368</v>
+        <v>357</v>
       </c>
       <c r="D11" s="46" t="s">
-        <v>369</v>
+        <v>358</v>
       </c>
       <c r="E11" s="44"/>
     </row>
     <row r="12" spans="1:5" s="43" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="43" t="s">
-        <v>394</v>
+        <v>382</v>
       </c>
       <c r="B12" s="46" t="s">
-        <v>390</v>
+        <v>378</v>
       </c>
       <c r="C12" s="46" t="s">
-        <v>370</v>
+        <v>359</v>
       </c>
       <c r="D12" s="46" t="s">
-        <v>371</v>
+        <v>360</v>
       </c>
       <c r="E12" s="46"/>
     </row>
@@ -3284,7 +3276,7 @@
         <v>85</v>
       </c>
       <c r="E14" s="31" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -3292,16 +3284,16 @@
         <v>55</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="D15" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="E15" s="34" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="43" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -3309,16 +3301,16 @@
         <v>55</v>
       </c>
       <c r="B16" s="46" t="s">
-        <v>409</v>
+        <v>397</v>
       </c>
       <c r="C16" s="46" t="s">
-        <v>410</v>
+        <v>398</v>
       </c>
       <c r="D16" s="43" t="s">
-        <v>411</v>
+        <v>399</v>
       </c>
       <c r="E16" s="45" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3326,16 +3318,16 @@
         <v>55</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="D17" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="E17" s="34" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
@@ -3343,16 +3335,16 @@
         <v>55</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="D18" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="E18" s="34" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
@@ -3360,16 +3352,16 @@
         <v>55</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="D19" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="E19" s="34" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
@@ -3383,10 +3375,10 @@
         <v>87</v>
       </c>
       <c r="D20" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="E20" s="34" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
@@ -3400,13 +3392,13 @@
         <v>46</v>
       </c>
       <c r="B23" s="46" t="s">
-        <v>353</v>
+        <v>342</v>
       </c>
       <c r="C23" s="46" t="s">
-        <v>354</v>
+        <v>343</v>
       </c>
       <c r="D23" s="43" t="s">
-        <v>355</v>
+        <v>344</v>
       </c>
       <c r="E23" s="46"/>
     </row>
@@ -3415,13 +3407,13 @@
         <v>46</v>
       </c>
       <c r="B24" s="46" t="s">
-        <v>356</v>
+        <v>345</v>
       </c>
       <c r="C24" s="46" t="s">
-        <v>357</v>
+        <v>346</v>
       </c>
       <c r="D24" s="46" t="s">
-        <v>358</v>
+        <v>347</v>
       </c>
       <c r="E24" s="46"/>
     </row>
@@ -3430,13 +3422,13 @@
         <v>46</v>
       </c>
       <c r="B25" s="46" t="s">
-        <v>359</v>
+        <v>348</v>
       </c>
       <c r="C25" s="46" t="s">
-        <v>360</v>
+        <v>349</v>
       </c>
       <c r="D25" s="46" t="s">
-        <v>361</v>
+        <v>350</v>
       </c>
       <c r="E25" s="46"/>
     </row>
@@ -3445,13 +3437,13 @@
         <v>46</v>
       </c>
       <c r="B26" s="46" t="s">
-        <v>362</v>
+        <v>351</v>
       </c>
       <c r="C26" s="46" t="s">
-        <v>363</v>
+        <v>352</v>
       </c>
       <c r="D26" s="43" t="s">
-        <v>364</v>
+        <v>353</v>
       </c>
       <c r="E26" s="46"/>
     </row>
@@ -3460,13 +3452,13 @@
         <v>46</v>
       </c>
       <c r="B27" s="46" t="s">
-        <v>365</v>
+        <v>354</v>
       </c>
       <c r="C27" s="46" t="s">
-        <v>366</v>
+        <v>355</v>
       </c>
       <c r="D27" s="43" t="s">
-        <v>367</v>
+        <v>356</v>
       </c>
       <c r="E27" s="46"/>
     </row>
@@ -3475,7 +3467,7 @@
     </row>
     <row r="30" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="B30" t="s">
         <v>89</v>
@@ -3487,12 +3479,12 @@
         <v>91</v>
       </c>
       <c r="E30" s="34" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="B31" t="s">
         <v>92</v>
@@ -3504,12 +3496,12 @@
         <v>93</v>
       </c>
       <c r="E31" s="34" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="B32" t="s">
         <v>80</v>
@@ -3521,7 +3513,7 @@
         <v>82</v>
       </c>
       <c r="E32" s="34" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
@@ -3638,7 +3630,7 @@
         <v>178</v>
       </c>
       <c r="E43" s="31" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -3655,7 +3647,7 @@
         <v>175</v>
       </c>
       <c r="E44" s="31" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -3672,7 +3664,7 @@
         <v>176</v>
       </c>
       <c r="E45" s="31" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -3689,7 +3681,7 @@
         <v>177</v>
       </c>
       <c r="E46" s="31" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -3706,7 +3698,7 @@
         <v>91</v>
       </c>
       <c r="E48" s="34" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -3714,7 +3706,7 @@
         <v>60</v>
       </c>
       <c r="B49" s="16" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="C49" s="16" t="s">
         <v>93</v>
@@ -3723,12 +3715,12 @@
         <v>93</v>
       </c>
       <c r="E49" s="34" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="16" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="B51" s="16" t="s">
         <v>89</v>
@@ -3740,12 +3732,12 @@
         <v>91</v>
       </c>
       <c r="E51" s="34" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="16" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="B52" s="16" t="s">
         <v>92</v>
@@ -3757,15 +3749,15 @@
         <v>93</v>
       </c>
       <c r="E52" s="34" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="16" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="B53" s="16" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="C53" s="16" t="s">
         <v>88</v>
@@ -3774,24 +3766,24 @@
         <v>88</v>
       </c>
       <c r="E53" s="34" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="16" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="C56" s="16" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="D56" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="E56" s="34" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
     </row>
   </sheetData>
@@ -3871,10 +3863,10 @@
         <v>119</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
@@ -3894,16 +3886,16 @@
         <v>118</v>
       </c>
       <c r="C3" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="D3" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="E3" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
@@ -4129,7 +4121,7 @@
         <v>7</v>
       </c>
       <c r="E1" s="37" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="F1" t="s">
         <v>145</v>
@@ -4138,7 +4130,7 @@
         <v>146</v>
       </c>
       <c r="H1" s="42" t="s">
-        <v>335</v>
+        <v>324</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="16.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4182,7 +4174,7 @@
         <v>153</v>
       </c>
       <c r="E5" s="38" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
       <c r="H5" s="41"/>
     </row>
@@ -4208,7 +4200,7 @@
         <v>157</v>
       </c>
       <c r="H7" s="42" t="s">
-        <v>332</v>
+        <v>321</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -4223,25 +4215,25 @@
         <v>160</v>
       </c>
       <c r="H8" s="42" t="s">
-        <v>333</v>
+        <v>322</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="39" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
       <c r="B9" s="39"/>
       <c r="C9" s="39"/>
       <c r="D9" s="39"/>
       <c r="E9" s="39"/>
       <c r="F9" s="40" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="G9" s="40" t="s">
-        <v>334</v>
+        <v>323</v>
       </c>
       <c r="H9" s="42" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
     </row>
   </sheetData>
@@ -4271,7 +4263,7 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -4287,7 +4279,7 @@
         <v>128</v>
       </c>
       <c r="B3" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="C3" t="b">
         <v>1</v>
@@ -4298,7 +4290,7 @@
         <v>128</v>
       </c>
       <c r="B4" s="41" t="s">
-        <v>395</v>
+        <v>383</v>
       </c>
       <c r="C4" s="41" t="b">
         <v>1</v>
@@ -4343,18 +4335,18 @@
     </row>
     <row r="2" spans="1:2" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>374</v>
+        <v>363</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>376</v>
+        <v>365</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="41" customFormat="1" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A3" s="41" t="s">
-        <v>375</v>
+        <v>364</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>377</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove picture from refrigerator form
</commit_message>
<xml_diff>
--- a/app/config/tables/refrigerators/forms/refrigerators/refrigerators.xlsx
+++ b/app/config/tables/refrigerators/forms/refrigerators/refrigerators.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="26940" windowHeight="13530" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="26940" windowHeight="13536" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="8" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="419">
   <si>
     <t>comments</t>
   </si>
@@ -1288,6 +1288,9 @@
   </si>
   <si>
     <t>Solo tome una foto si es necesario para la verificación</t>
+  </si>
+  <si>
+    <t>(false)</t>
   </si>
 </sst>
 </file>
@@ -1921,16 +1924,16 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.54296875" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.5546875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.453125" style="50" customWidth="1"/>
-    <col min="2" max="2" width="9.54296875" style="50"/>
-    <col min="3" max="3" width="19.54296875" style="50" customWidth="1"/>
-    <col min="4" max="4" width="26.453125" style="50" customWidth="1"/>
-    <col min="5" max="16384" width="9.54296875" style="50"/>
+    <col min="1" max="1" width="17.44140625" style="50" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" style="50"/>
+    <col min="3" max="3" width="19.5546875" style="50" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" style="50" customWidth="1"/>
+    <col min="5" max="16384" width="9.5546875" style="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="49" t="s">
         <v>1</v>
       </c>
@@ -1944,14 +1947,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="49" t="s">
         <v>385</v>
       </c>
       <c r="B2" s="49"/>
       <c r="C2" s="49"/>
     </row>
-    <row r="3" spans="1:4" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="78" x14ac:dyDescent="0.3">
       <c r="A3" s="49" t="s">
         <v>386</v>
       </c>
@@ -1969,27 +1972,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V63"/>
+  <dimension ref="A1:V65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M2" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="X26" sqref="X26"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.81640625" customWidth="1"/>
-    <col min="2" max="3" width="11.453125" customWidth="1"/>
-    <col min="4" max="4" width="20.453125" customWidth="1"/>
-    <col min="5" max="5" width="42.453125" customWidth="1"/>
-    <col min="6" max="6" width="24.54296875" customWidth="1"/>
-    <col min="7" max="7" width="29.54296875" customWidth="1"/>
-    <col min="8" max="9" width="30.453125" customWidth="1"/>
-    <col min="10" max="10" width="41.54296875" customWidth="1"/>
-    <col min="11" max="12" width="22.81640625" customWidth="1"/>
-    <col min="13" max="13" width="19.54296875" customWidth="1"/>
-    <col min="14" max="15" width="20.26953125" customWidth="1"/>
-    <col min="16" max="16" width="16.1796875" customWidth="1"/>
-    <col min="17" max="1029" width="11.453125" customWidth="1"/>
+    <col min="1" max="1" width="42.77734375" customWidth="1"/>
+    <col min="2" max="3" width="11.44140625" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" customWidth="1"/>
+    <col min="5" max="5" width="42.44140625" customWidth="1"/>
+    <col min="6" max="6" width="24.5546875" customWidth="1"/>
+    <col min="7" max="7" width="29.5546875" customWidth="1"/>
+    <col min="8" max="9" width="30.44140625" customWidth="1"/>
+    <col min="10" max="10" width="41.5546875" customWidth="1"/>
+    <col min="11" max="12" width="22.77734375" customWidth="1"/>
+    <col min="13" max="13" width="19.5546875" customWidth="1"/>
+    <col min="14" max="15" width="20.21875" customWidth="1"/>
+    <col min="16" max="16" width="16.21875" customWidth="1"/>
+    <col min="17" max="1029" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
@@ -2060,7 +2063,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>15</v>
       </c>
@@ -2091,7 +2094,7 @@
       <c r="U3" s="3"/>
       <c r="V3" s="3"/>
     </row>
-    <row r="4" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>16</v>
       </c>
@@ -2101,7 +2104,7 @@
       <c r="I4" s="17"/>
       <c r="L4" s="23"/>
     </row>
-    <row r="5" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>18</v>
       </c>
@@ -2154,7 +2157,7 @@
       <c r="D7" s="3"/>
       <c r="P7" s="6"/>
     </row>
-    <row r="8" spans="1:22" s="41" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" s="41" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" s="3" t="s">
         <v>24</v>
       </c>
@@ -2183,7 +2186,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="9" spans="1:22" s="41" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" s="41" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="41" t="s">
         <v>23</v>
       </c>
@@ -2302,7 +2305,7 @@
       <c r="D17" s="3"/>
       <c r="P17" s="6"/>
     </row>
-    <row r="18" spans="1:22" s="41" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" s="41" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D18" s="3" t="s">
         <v>24</v>
       </c>
@@ -2334,7 +2337,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>30</v>
       </c>
@@ -2343,7 +2346,7 @@
       <c r="I19" s="17"/>
       <c r="L19" s="23"/>
     </row>
-    <row r="20" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>23</v>
       </c>
@@ -2352,14 +2355,14 @@
       <c r="I20" s="17"/>
       <c r="L20" s="23"/>
     </row>
-    <row r="21" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>15</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D22" s="3" t="s">
         <v>33</v>
       </c>
@@ -2386,7 +2389,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="23" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D23" s="3" t="s">
         <v>179</v>
       </c>
@@ -2428,7 +2431,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="24" spans="1:22" s="43" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" s="43" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D24" s="44" t="s">
         <v>179</v>
       </c>
@@ -2470,649 +2473,672 @@
         <v>413</v>
       </c>
     </row>
-    <row r="25" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>30</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="1:22" s="43" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D26" s="45" t="s">
+    <row r="26" spans="1:22" s="41" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="41" t="s">
+        <v>216</v>
+      </c>
+      <c r="C26" s="41" t="s">
+        <v>418</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:22" s="43" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D27" s="45" t="s">
         <v>231</v>
       </c>
-      <c r="E26" s="44"/>
-      <c r="F26" s="45" t="s">
+      <c r="E27" s="44"/>
+      <c r="F27" s="45" t="s">
         <v>327</v>
       </c>
-      <c r="G26" s="45" t="s">
+      <c r="G27" s="45" t="s">
         <v>322</v>
       </c>
-      <c r="H26" s="45" t="s">
+      <c r="H27" s="45" t="s">
         <v>328</v>
       </c>
-      <c r="J26" s="45" t="s">
+      <c r="J27" s="45" t="s">
         <v>329</v>
       </c>
-      <c r="K26" s="45" t="s">
+      <c r="K27" s="45" t="s">
         <v>330</v>
       </c>
-      <c r="L26" s="45"/>
-      <c r="M26" s="43" t="s">
+      <c r="L27" s="45"/>
+      <c r="M27" s="43" t="s">
         <v>416</v>
       </c>
-      <c r="N26" s="43" t="s">
+      <c r="N27" s="43" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="27" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D27" s="3" t="s">
+    <row r="28" spans="1:22" s="42" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" s="34"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="34"/>
+      <c r="J28" s="34"/>
+      <c r="K28" s="34"/>
+      <c r="L28" s="34"/>
+    </row>
+    <row r="29" spans="1:22" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D29" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E27" s="3"/>
-      <c r="F27" t="s">
+      <c r="E29" s="3"/>
+      <c r="F29" t="s">
         <v>185</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G29" t="s">
         <v>186</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H29" t="s">
         <v>187</v>
       </c>
-      <c r="I27" s="18" t="s">
+      <c r="I29" s="18" t="s">
         <v>262</v>
       </c>
-      <c r="J27" t="s">
+      <c r="J29" t="s">
         <v>188</v>
       </c>
-      <c r="K27" t="s">
+      <c r="K29" t="s">
         <v>189</v>
       </c>
-      <c r="L27" s="24" t="s">
+      <c r="L29" s="24" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="28" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+    <row r="30" spans="1:22" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
         <v>15</v>
-      </c>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="I28" s="17"/>
-      <c r="L28" s="23"/>
-    </row>
-    <row r="29" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E29" s="16" t="s">
-        <v>224</v>
-      </c>
-      <c r="F29" t="s">
-        <v>190</v>
-      </c>
-      <c r="G29" t="s">
-        <v>191</v>
-      </c>
-      <c r="H29" t="s">
-        <v>193</v>
-      </c>
-      <c r="I29" s="18" t="s">
-        <v>264</v>
-      </c>
-      <c r="J29" t="s">
-        <v>192</v>
-      </c>
-      <c r="K29" t="s">
-        <v>194</v>
-      </c>
-      <c r="L29" s="24" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="30" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>16</v>
-      </c>
-      <c r="C30" t="s">
-        <v>195</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="I30" s="17"/>
       <c r="L30" s="23"/>
     </row>
-    <row r="31" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D31" t="s">
+    <row r="31" spans="1:22" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D31" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="F31" t="s">
+        <v>190</v>
+      </c>
+      <c r="G31" t="s">
+        <v>191</v>
+      </c>
+      <c r="H31" t="s">
+        <v>193</v>
+      </c>
+      <c r="I31" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="J31" t="s">
+        <v>192</v>
+      </c>
+      <c r="K31" t="s">
+        <v>194</v>
+      </c>
+      <c r="L31" s="24" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" t="s">
+        <v>195</v>
+      </c>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="I32" s="17"/>
+      <c r="L32" s="23"/>
+    </row>
+    <row r="33" spans="2:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
         <v>33</v>
       </c>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3" t="s">
+      <c r="E33" s="3"/>
+      <c r="F33" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G33" t="s">
         <v>198</v>
       </c>
-      <c r="H31" t="s">
+      <c r="H33" t="s">
         <v>199</v>
       </c>
-      <c r="I31" s="20" t="s">
+      <c r="I33" s="20" t="s">
         <v>265</v>
       </c>
-      <c r="J31" t="s">
+      <c r="J33" t="s">
         <v>200</v>
       </c>
-      <c r="K31" t="s">
+      <c r="K33" t="s">
         <v>201</v>
       </c>
-      <c r="L31" s="25" t="s">
+      <c r="L33" s="25" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="32" spans="1:22" s="43" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D32" s="44" t="s">
+    <row r="34" spans="2:12" s="43" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D34" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="E32" s="44"/>
-      <c r="F32" s="43" t="s">
+      <c r="E34" s="44"/>
+      <c r="F34" s="43" t="s">
         <v>197</v>
       </c>
-      <c r="G32" s="43" t="s">
+      <c r="G34" s="43" t="s">
         <v>394</v>
       </c>
-      <c r="H32" s="43" t="s">
+      <c r="H34" s="43" t="s">
         <v>395</v>
       </c>
-      <c r="I32" s="53" t="s">
+      <c r="I34" s="53" t="s">
         <v>266</v>
       </c>
-      <c r="J32" s="43" t="s">
+      <c r="J34" s="43" t="s">
         <v>396</v>
       </c>
-      <c r="K32" s="43" t="s">
+      <c r="K34" s="43" t="s">
         <v>397</v>
       </c>
-      <c r="L32" s="53" t="s">
+      <c r="L34" s="53" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="33" spans="2:12" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
+    <row r="35" spans="2:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
         <v>23</v>
-      </c>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="I33" s="17"/>
-      <c r="L33" s="23"/>
-    </row>
-    <row r="34" spans="2:12" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>30</v>
-      </c>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="I34" s="17"/>
-      <c r="L34" s="23"/>
-    </row>
-    <row r="35" spans="2:12" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>15</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
       <c r="I35" s="17"/>
       <c r="L35" s="23"/>
     </row>
-    <row r="36" spans="2:12" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D36" t="s">
-        <v>24</v>
-      </c>
-      <c r="E36" t="s">
-        <v>41</v>
-      </c>
-      <c r="F36" t="s">
-        <v>42</v>
-      </c>
-      <c r="G36" t="s">
-        <v>43</v>
-      </c>
-      <c r="H36" t="s">
-        <v>44</v>
-      </c>
-      <c r="I36" s="18" t="s">
-        <v>267</v>
-      </c>
-      <c r="J36" t="s">
-        <v>45</v>
-      </c>
-      <c r="K36" t="s">
-        <v>44</v>
-      </c>
-      <c r="L36" s="24" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="37" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D37" t="s">
-        <v>24</v>
-      </c>
-      <c r="E37" t="s">
-        <v>46</v>
-      </c>
-      <c r="F37" t="s">
-        <v>47</v>
-      </c>
-      <c r="G37" t="s">
-        <v>48</v>
-      </c>
-      <c r="H37" t="s">
-        <v>49</v>
-      </c>
-      <c r="I37" s="18" t="s">
-        <v>268</v>
-      </c>
-      <c r="J37" t="s">
-        <v>50</v>
-      </c>
-      <c r="K37" t="s">
-        <v>51</v>
-      </c>
-      <c r="L37" s="26" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="38" spans="2:12" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>30</v>
+      </c>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="I36" s="17"/>
+      <c r="L36" s="23"/>
+    </row>
+    <row r="37" spans="2:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="I37" s="17"/>
+      <c r="L37" s="23"/>
+    </row>
+    <row r="38" spans="2:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
         <v>24</v>
       </c>
       <c r="E38" t="s">
-        <v>376</v>
+        <v>41</v>
       </c>
       <c r="F38" t="s">
-        <v>204</v>
+        <v>42</v>
       </c>
       <c r="G38" t="s">
-        <v>202</v>
+        <v>43</v>
       </c>
       <c r="H38" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="I38" s="18" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="J38" t="s">
-        <v>203</v>
+        <v>45</v>
       </c>
       <c r="K38" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="L38" s="24" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="39" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D39" s="14" t="s">
-        <v>217</v>
+      <c r="D39" t="s">
+        <v>24</v>
       </c>
       <c r="E39" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="F39" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="G39" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="H39" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="I39" s="18" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="J39" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="K39" t="s">
-        <v>58</v>
-      </c>
-      <c r="L39" s="24" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="40" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="L39" s="26" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
         <v>24</v>
       </c>
       <c r="E40" t="s">
+        <v>376</v>
+      </c>
+      <c r="F40" t="s">
+        <v>204</v>
+      </c>
+      <c r="G40" t="s">
+        <v>202</v>
+      </c>
+      <c r="H40" t="s">
+        <v>53</v>
+      </c>
+      <c r="I40" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="J40" t="s">
+        <v>203</v>
+      </c>
+      <c r="K40" t="s">
+        <v>54</v>
+      </c>
+      <c r="L40" s="24" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D41" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="E41" t="s">
+        <v>55</v>
+      </c>
+      <c r="F41" t="s">
+        <v>56</v>
+      </c>
+      <c r="G41" t="s">
+        <v>57</v>
+      </c>
+      <c r="H41" t="s">
+        <v>58</v>
+      </c>
+      <c r="I41" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="J41" t="s">
+        <v>59</v>
+      </c>
+      <c r="K41" t="s">
+        <v>58</v>
+      </c>
+      <c r="L41" s="24" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>24</v>
+      </c>
+      <c r="E42" t="s">
         <v>163</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F42" t="s">
         <v>164</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G42" t="s">
         <v>165</v>
       </c>
-      <c r="H40" t="s">
+      <c r="H42" t="s">
         <v>166</v>
       </c>
-      <c r="I40" s="18" t="s">
+      <c r="I42" s="18" t="s">
         <v>271</v>
       </c>
-      <c r="J40" t="s">
+      <c r="J42" t="s">
         <v>167</v>
       </c>
-      <c r="K40" t="s">
+      <c r="K42" t="s">
         <v>168</v>
       </c>
-      <c r="L40" s="28" t="s">
+      <c r="L42" s="28" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="41" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
+    <row r="43" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
         <v>30</v>
-      </c>
-      <c r="I41" s="17"/>
-      <c r="L41" s="23"/>
-    </row>
-    <row r="42" spans="2:12" s="41" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="C42" s="41" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>15</v>
       </c>
       <c r="I43" s="17"/>
       <c r="L43" s="23"/>
     </row>
-    <row r="44" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D44" t="s">
-        <v>24</v>
-      </c>
-      <c r="E44" s="16" t="s">
-        <v>226</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G44" t="s">
-        <v>62</v>
-      </c>
-      <c r="H44" t="s">
-        <v>63</v>
-      </c>
-      <c r="I44" s="19" t="s">
-        <v>272</v>
-      </c>
-      <c r="J44" t="s">
-        <v>64</v>
-      </c>
-      <c r="K44" t="s">
-        <v>65</v>
-      </c>
-      <c r="L44" s="26" t="s">
-        <v>289</v>
+    <row r="44" spans="2:12" s="41" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="C44" s="41" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>16</v>
-      </c>
-      <c r="C45" t="s">
-        <v>205</v>
+        <v>15</v>
       </c>
       <c r="I45" s="17"/>
       <c r="L45" s="23"/>
     </row>
-    <row r="46" spans="2:12" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D46" s="43" t="s">
+    <row r="46" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>24</v>
+      </c>
+      <c r="E46" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G46" t="s">
+        <v>62</v>
+      </c>
+      <c r="H46" t="s">
+        <v>63</v>
+      </c>
+      <c r="I46" s="19" t="s">
+        <v>272</v>
+      </c>
+      <c r="J46" t="s">
+        <v>64</v>
+      </c>
+      <c r="K46" t="s">
+        <v>65</v>
+      </c>
+      <c r="L46" s="26" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>16</v>
+      </c>
+      <c r="C47" t="s">
+        <v>205</v>
+      </c>
+      <c r="I47" s="17"/>
+      <c r="L47" s="23"/>
+    </row>
+    <row r="48" spans="2:12" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D48" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="F46" s="43" t="s">
+      <c r="F48" s="43" t="s">
         <v>399</v>
       </c>
-      <c r="G46" s="43" t="s">
+      <c r="G48" s="43" t="s">
         <v>400</v>
       </c>
-      <c r="H46" s="43" t="s">
+      <c r="H48" s="43" t="s">
         <v>401</v>
       </c>
-      <c r="J46" s="43" t="s">
+      <c r="J48" s="43" t="s">
         <v>402</v>
       </c>
-      <c r="K46" s="43" t="s">
+      <c r="K48" s="43" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="47" spans="2:12" ht="25" x14ac:dyDescent="0.25">
-      <c r="D47" t="s">
+    <row r="49" spans="2:12" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
         <v>24</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E49" t="s">
         <v>52</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F49" t="s">
         <v>207</v>
       </c>
-      <c r="G47" t="s">
+      <c r="G49" t="s">
         <v>206</v>
       </c>
-      <c r="H47" t="s">
+      <c r="H49" t="s">
         <v>208</v>
       </c>
-      <c r="I47" s="22" t="s">
+      <c r="I49" s="22" t="s">
         <v>273</v>
       </c>
-      <c r="J47" t="s">
+      <c r="J49" t="s">
         <v>209</v>
       </c>
-      <c r="K47" t="s">
+      <c r="K49" t="s">
         <v>210</v>
       </c>
-      <c r="L47" s="29" t="s">
+      <c r="L49" s="29" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
+    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
         <v>23</v>
       </c>
-      <c r="I48" s="17"/>
-      <c r="L48" s="23"/>
-    </row>
-    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>30</v>
-      </c>
-      <c r="I49" s="17"/>
-      <c r="L49" s="23"/>
-    </row>
-    <row r="50" spans="2:12" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="41" t="s">
-        <v>23</v>
-      </c>
+      <c r="I50" s="17"/>
+      <c r="L50" s="23"/>
     </row>
     <row r="51" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="I51" s="17"/>
       <c r="L51" s="23"/>
     </row>
-    <row r="52" spans="2:12" ht="25" x14ac:dyDescent="0.25">
-      <c r="D52" t="s">
-        <v>24</v>
-      </c>
-      <c r="E52" t="s">
-        <v>60</v>
-      </c>
-      <c r="F52" t="s">
-        <v>211</v>
-      </c>
-      <c r="G52" t="s">
-        <v>212</v>
-      </c>
-      <c r="H52" t="s">
-        <v>213</v>
-      </c>
-      <c r="I52" s="22" t="s">
-        <v>274</v>
-      </c>
-      <c r="J52" t="s">
-        <v>214</v>
-      </c>
-      <c r="K52" t="s">
-        <v>215</v>
-      </c>
-      <c r="L52" s="26" t="s">
-        <v>291</v>
+    <row r="52" spans="2:12" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="41" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="53" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>216</v>
-      </c>
-      <c r="C53" t="s">
-        <v>363</v>
+        <v>15</v>
       </c>
       <c r="I53" s="17"/>
       <c r="L53" s="23"/>
     </row>
-    <row r="54" spans="2:12" ht="25" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:12" ht="26.4" x14ac:dyDescent="0.25">
       <c r="D54" t="s">
+        <v>24</v>
+      </c>
+      <c r="E54" t="s">
+        <v>60</v>
+      </c>
+      <c r="F54" t="s">
+        <v>211</v>
+      </c>
+      <c r="G54" t="s">
+        <v>212</v>
+      </c>
+      <c r="H54" t="s">
+        <v>213</v>
+      </c>
+      <c r="I54" s="22" t="s">
+        <v>274</v>
+      </c>
+      <c r="J54" t="s">
+        <v>214</v>
+      </c>
+      <c r="K54" t="s">
+        <v>215</v>
+      </c>
+      <c r="L54" s="26" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>216</v>
+      </c>
+      <c r="C55" t="s">
+        <v>363</v>
+      </c>
+      <c r="I55" s="17"/>
+      <c r="L55" s="23"/>
+    </row>
+    <row r="56" spans="2:12" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="D56" t="s">
         <v>33</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F56" t="s">
         <v>219</v>
       </c>
-      <c r="G54" t="s">
+      <c r="G56" t="s">
         <v>220</v>
       </c>
-      <c r="H54" t="s">
+      <c r="H56" t="s">
         <v>221</v>
       </c>
-      <c r="I54" s="22" t="s">
+      <c r="I56" s="22" t="s">
         <v>275</v>
       </c>
-      <c r="J54" t="s">
+      <c r="J56" t="s">
         <v>222</v>
       </c>
-      <c r="K54" t="s">
+      <c r="K56" t="s">
         <v>223</v>
       </c>
-      <c r="L54" s="26" t="s">
+      <c r="L56" s="26" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="55" spans="2:12" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D55" s="41" t="s">
+    <row r="57" spans="2:12" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D57" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="E55" s="41" t="s">
+      <c r="E57" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="F55" s="41" t="s">
+      <c r="F57" s="41" t="s">
         <v>364</v>
       </c>
-      <c r="G55" s="41" t="s">
+      <c r="G57" s="41" t="s">
         <v>365</v>
       </c>
-      <c r="H55" s="41" t="s">
+      <c r="H57" s="41" t="s">
         <v>366</v>
       </c>
-      <c r="I55" s="28"/>
-      <c r="J55" s="41" t="s">
+      <c r="I57" s="28"/>
+      <c r="J57" s="41" t="s">
         <v>367</v>
       </c>
-      <c r="K55" s="41" t="s">
+      <c r="K57" s="41" t="s">
         <v>368</v>
       </c>
-      <c r="L55" s="34"/>
-    </row>
-    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
+      <c r="L57" s="34"/>
+    </row>
+    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
         <v>23</v>
       </c>
-      <c r="I56" s="17"/>
-      <c r="L56" s="23"/>
-    </row>
-    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
+      <c r="I58" s="17"/>
+      <c r="L58" s="23"/>
+    </row>
+    <row r="59" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
         <v>30</v>
       </c>
-      <c r="I57" s="17"/>
-      <c r="L57" s="23"/>
-    </row>
-    <row r="58" spans="2:12" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="41" t="s">
+      <c r="I59" s="17"/>
+      <c r="L59" s="23"/>
+    </row>
+    <row r="60" spans="2:12" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="C58" s="41" t="s">
+      <c r="C60" s="41" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="59" spans="2:12" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="41" t="s">
+    <row r="61" spans="2:12" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="41" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="2:12" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D60" s="43" t="s">
+    <row r="62" spans="2:12" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D62" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="E60" s="43" t="s">
+      <c r="E62" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="F60" s="43" t="s">
+      <c r="F62" s="43" t="s">
         <v>334</v>
       </c>
-      <c r="G60" s="43" t="s">
+      <c r="G62" s="43" t="s">
         <v>335</v>
       </c>
-      <c r="H60" s="43" t="s">
+      <c r="H62" s="43" t="s">
         <v>336</v>
       </c>
-      <c r="J60" s="43" t="s">
+      <c r="J62" s="43" t="s">
         <v>333</v>
       </c>
-      <c r="K60" s="43" t="s">
+      <c r="K62" s="43" t="s">
         <v>337</v>
       </c>
-      <c r="L60" s="45"/>
-    </row>
-    <row r="61" spans="2:12" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="42" t="s">
+      <c r="L62" s="45"/>
+    </row>
+    <row r="63" spans="2:12" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="L61" s="34"/>
-    </row>
-    <row r="62" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
+      <c r="L63" s="34"/>
+    </row>
+    <row r="64" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="63" spans="2:12" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D63" s="43" t="s">
+    <row r="65" spans="4:11" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D65" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="F63" s="43" t="s">
+      <c r="F65" s="43" t="s">
         <v>404</v>
       </c>
-      <c r="G63" s="43" t="s">
+      <c r="G65" s="43" t="s">
         <v>405</v>
       </c>
-      <c r="H63" s="43" t="s">
+      <c r="H65" s="43" t="s">
         <v>407</v>
       </c>
-      <c r="J63" s="43" t="s">
+      <c r="J65" s="43" t="s">
         <v>406</v>
       </c>
-      <c r="K63" s="43" t="s">
+      <c r="K65" s="43" t="s">
         <v>408</v>
       </c>
     </row>
@@ -3130,17 +3156,17 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.54296875" customWidth="1"/>
-    <col min="2" max="2" width="33.54296875" customWidth="1"/>
-    <col min="3" max="3" width="28.453125" customWidth="1"/>
-    <col min="4" max="4" width="20.1796875" customWidth="1"/>
+    <col min="1" max="1" width="18.5546875" customWidth="1"/>
+    <col min="2" max="2" width="33.5546875" customWidth="1"/>
+    <col min="3" max="3" width="28.44140625" customWidth="1"/>
+    <col min="4" max="4" width="20.21875" customWidth="1"/>
     <col min="5" max="5" width="27" customWidth="1"/>
-    <col min="6" max="1025" width="8.54296875" customWidth="1"/>
+    <col min="6" max="1025" width="8.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>66</v>
       </c>
@@ -3157,7 +3183,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="4" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="4" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>41</v>
       </c>
@@ -3174,7 +3200,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="4" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="4" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>41</v>
       </c>
@@ -3191,7 +3217,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="4" customFormat="1" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="4" customFormat="1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>41</v>
       </c>
@@ -3208,7 +3234,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="4" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>41</v>
       </c>
@@ -3225,7 +3251,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="4" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" s="4" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -3242,7 +3268,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="4" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" s="4" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -3265,7 +3291,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="41" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" s="41" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="41" t="s">
         <v>52</v>
       </c>
@@ -3297,7 +3323,7 @@
       </c>
       <c r="E11" s="44"/>
     </row>
-    <row r="12" spans="1:5" s="43" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" s="43" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="43" t="s">
         <v>376</v>
       </c>
@@ -3312,7 +3338,7 @@
       </c>
       <c r="E12" s="46"/>
     </row>
-    <row r="14" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>55</v>
       </c>
@@ -3329,7 +3355,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>55</v>
       </c>
@@ -3346,7 +3372,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="43" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" s="43" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="43" t="s">
         <v>55</v>
       </c>
@@ -3380,7 +3406,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>55</v>
       </c>
@@ -3397,7 +3423,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -3414,7 +3440,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>55</v>
       </c>
@@ -3431,7 +3457,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16"/>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
@@ -3515,7 +3541,7 @@
     <row r="28" spans="1:5" s="41" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E28" s="34"/>
     </row>
-    <row r="30" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
         <v>224</v>
       </c>
@@ -3532,7 +3558,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
         <v>224</v>
       </c>
@@ -3549,7 +3575,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
         <v>224</v>
       </c>
@@ -3566,7 +3592,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>25</v>
       </c>
@@ -3583,7 +3609,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>25</v>
       </c>
@@ -3850,21 +3876,21 @@
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.81640625" customWidth="1"/>
-    <col min="2" max="2" width="21.453125" customWidth="1"/>
-    <col min="3" max="3" width="17.81640625" customWidth="1"/>
-    <col min="4" max="4" width="19.453125" customWidth="1"/>
-    <col min="5" max="5" width="17.453125" customWidth="1"/>
-    <col min="6" max="6" width="19.453125" customWidth="1"/>
-    <col min="7" max="9" width="39.54296875" customWidth="1"/>
-    <col min="10" max="10" width="39.453125" customWidth="1"/>
+    <col min="1" max="1" width="22.77734375" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" customWidth="1"/>
+    <col min="3" max="3" width="17.77734375" customWidth="1"/>
+    <col min="4" max="4" width="19.44140625" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" customWidth="1"/>
+    <col min="6" max="6" width="19.44140625" customWidth="1"/>
+    <col min="7" max="9" width="39.5546875" customWidth="1"/>
+    <col min="10" max="10" width="39.44140625" customWidth="1"/>
     <col min="11" max="11" width="43" customWidth="1"/>
-    <col min="12" max="1025" width="10.81640625" customWidth="1"/>
+    <col min="12" max="1025" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>107</v>
       </c>
@@ -3899,7 +3925,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>29</v>
       </c>
@@ -3928,7 +3954,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -3976,14 +4002,14 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="10.81640625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="34.453125" style="11" customWidth="1"/>
-    <col min="4" max="1025" width="10.81640625" style="11" customWidth="1"/>
+    <col min="1" max="2" width="10.77734375" style="11" customWidth="1"/>
+    <col min="3" max="3" width="34.44140625" style="11" customWidth="1"/>
+    <col min="4" max="1025" width="10.77734375" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>121</v>
       </c>
@@ -4000,7 +4026,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>125</v>
       </c>
@@ -4017,7 +4043,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>125</v>
       </c>
@@ -4034,7 +4060,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>125</v>
       </c>
@@ -4051,7 +4077,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>125</v>
       </c>
@@ -4068,7 +4094,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>125</v>
       </c>
@@ -4085,14 +4111,14 @@
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
       <c r="E7" s="12"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>138</v>
       </c>
@@ -4109,7 +4135,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>141</v>
       </c>
@@ -4145,19 +4171,19 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="17.54296875" customWidth="1"/>
-    <col min="4" max="4" width="17.81640625" customWidth="1"/>
-    <col min="5" max="5" width="19.1796875" style="30" customWidth="1"/>
-    <col min="6" max="6" width="15.7265625" customWidth="1"/>
-    <col min="7" max="7" width="19.26953125" customWidth="1"/>
-    <col min="8" max="1026" width="11.453125" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" customWidth="1"/>
+    <col min="4" max="4" width="17.77734375" customWidth="1"/>
+    <col min="5" max="5" width="19.21875" style="30" customWidth="1"/>
+    <col min="6" max="6" width="15.77734375" customWidth="1"/>
+    <col min="7" max="7" width="19.21875" customWidth="1"/>
+    <col min="8" max="1026" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>144</v>
       </c>
@@ -4183,7 +4209,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="16.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>147</v>
       </c>
@@ -4193,7 +4219,7 @@
       <c r="E2" s="36"/>
       <c r="H2" s="41"/>
     </row>
-    <row r="3" spans="1:8" ht="16.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>149</v>
       </c>
@@ -4203,7 +4229,7 @@
       <c r="E3" s="36"/>
       <c r="H3" s="41"/>
     </row>
-    <row r="4" spans="1:8" ht="16.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>150</v>
       </c>
@@ -4213,7 +4239,7 @@
       <c r="E4" s="36"/>
       <c r="H4" s="41"/>
     </row>
-    <row r="5" spans="1:8" ht="16.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>151</v>
       </c>
@@ -4300,9 +4326,9 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="33.453125" customWidth="1"/>
+    <col min="2" max="2" width="33.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -4369,10 +4395,10 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.453125" customWidth="1"/>
-    <col min="2" max="2" width="42.81640625" customWidth="1"/>
+    <col min="1" max="1" width="34.44140625" customWidth="1"/>
+    <col min="2" max="2" width="42.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -4383,7 +4409,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="112.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>359</v>
       </c>
@@ -4391,7 +4417,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="41" customFormat="1" ht="137.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" s="41" customFormat="1" ht="145.19999999999999" x14ac:dyDescent="0.25">
       <c r="A3" s="41" t="s">
         <v>360</v>
       </c>

</xml_diff>